<commit_message>
I'll try one last time today to make binder work...
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -17683,8 +17683,8 @@
   <dimension ref="A1:R505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Trying binder again, this time I updated my R version to 4.4.1
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit mit bindr/Markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E393744-EC01-45F0-B629-2F55E497D0F8}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF11A221-BCCF-44C2-AC5E-48BC80A5EDBE}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="107">
   <si>
     <t>@article{example2024,   title = {A Reference Example},   journal = {Journal of Examples},   publisher = {Example Press},   author = {Doe, Jane},   year = {2024},   month = aug,   pages = {185–209} }</t>
   </si>
@@ -483,6 +483,24 @@
   </si>
   <si>
     <t xml:space="preserve">PA = körperliche Aktivität </t>
+  </si>
+  <si>
+    <t>@incollection{Ainsworth2020,
+  author = {Ainsworth, Barbara E. and Der Ananian, Cheryl},
+  title = {Physical Activity Promotion},
+  booktitle = {Handbook of Sport Psychology},
+  editor = {Tenenbaum, Gershon and Eklund, Robert C.},
+  volume = {II},
+  edition = {4th},
+  year = {2020},
+  publisher = {John Wiley \&amp; Sons, Inc.},
+  address = {Hoboken, NJ},
+  pages = {xx--xx},
+  doi = {https://doi.org/10.1002/9781119568124.ch37}
+}</t>
+  </si>
+  <si>
+    <t>dEFINITIONvon Bewegungsförderung, auch viele Studien auf Seite 810 zum Bewegungsmangel</t>
   </si>
   <si>
     <t>Abbreviations</t>
@@ -17683,8 +17701,8 @@
   <dimension ref="A1:R505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D32" sqref="D32"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -18652,36 +18670,41 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="36" customHeight="1">
-      <c r="A26" s="17"/>
+      <c r="A26" s="17" t="s">
+        <v>59</v>
+      </c>
       <c r="B26" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@Ainsworth2020</v>
       </c>
       <c r="C26" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@Ainsworth2020]</v>
       </c>
       <c r="D26" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2020</v>
       </c>
       <c r="E26" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Ainsworth, Barbara E. and Der Ananian, Cheryl</v>
       </c>
       <c r="F26" s="12" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>Physical Activity Promotion</v>
       </c>
       <c r="G26" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H26" s="15" t="str">
+        <v>https://doi.org/https://doi.org/10.1002/9781119568124.ch37</v>
+      </c>
+      <c r="H26" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45589.89381238426</v>
       </c>
       <c r="I26" s="1"/>
+      <c r="K26" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="36" customHeight="1">
       <c r="A27" s="17"/>
@@ -33980,15 +34003,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -34013,176 +34036,176 @@
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="72.75" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="23" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="180" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="210" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="255" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="255" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="285" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="285" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105" customHeight="1">
       <c r="A19" s="25" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120" customHeight="1">
       <c r="A20" s="25" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135" customHeight="1">
       <c r="A21" s="25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I elaborated on the mental health benefits of exercise
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit mit bindr/Markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{837F3C36-A8B6-4C54-8131-C0C91983DB06}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17E49C7D-EDDC-47D4-BF17-AEBBFCAD6101}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="126">
   <si>
     <t>@article{example2024,   title = {A Reference Example},   journal = {Journal of Examples},   publisher = {Example Press},   author = {Doe, Jane},   year = {2024},   month = aug,   pages = {185–209} }</t>
   </si>
@@ -629,6 +629,58 @@
   </si>
   <si>
     <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/PIIS0140673612610319.pdf?csf=1&amp;web=1&amp;e=veeVmS</t>
+  </si>
+  <si>
+    <t>@article{Paluska2000,
+  title = {Physical Activity and Mental Health: Current Concepts},
+  volume = {29},
+  ISSN = {0112-1642},
+  url = {http://dx.doi.org/10.2165/00007256-200029030-00003},
+  DOI = {10.2165/00007256-200029030-00003},
+  number = {3},
+  journal = {Sports Medicine},
+  publisher = {Springer Science and Business Media LLC},
+  author = {Paluska,  Scott A. and Schwenk,  Thomas L.},
+  year = {2000},
+  pages = {167–180}
+}</t>
+  </si>
+  <si>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/00007256-200029030-00003.pdf?csf=1&amp;web=1&amp;e=RdUDtc</t>
+  </si>
+  <si>
+    <t>@article{Mikkelsen2017,
+  title = {Exercise and mental health},
+  volume = {106},
+  ISSN = {0378-5122},
+  url = {http://dx.doi.org/10.1016/j.maturitas.2017.09.003},
+  DOI = {10.1016/j.maturitas.2017.09.003},
+  journal = {Maturitas},
+  publisher = {Elsevier BV},
+  author = {Mikkelsen,  Kathleen and Stojanovska,  Lily and Polenakovic,  Momir and Bosevski,  Marijan and Apostolopoulos,  Vasso},
+  year = {2017},
+  month = dec,
+  pages = {48–56}
+}</t>
+  </si>
+  <si>
+    <t>Exercise hat vor allem viele Vorteile</t>
+  </si>
+  <si>
+    <t>@article{Carter2016,
+  title = {The Effect of Exercise on Depressive Symptoms in Adolescents: A Systematic Review and Meta-Analysis},
+  volume = {55},
+  ISSN = {0890-8567},
+  url = {http://dx.doi.org/10.1016/j.jaac.2016.04.016},
+  DOI = {10.1016/j.jaac.2016.04.016},
+  number = {7},
+  journal = {Journal of the American Academy of Child &amp;amp; Adolescent Psychiatry},
+  publisher = {Elsevier BV},
+  author = {Carter,  Tim and Morres,  Ioannis D. and Meade,  Oonagh and Callaghan,  Patrick},
+  year = {2016},
+  month = jul,
+  pages = {580–590}
+}</t>
   </si>
   <si>
     <t>Abbreviations</t>
@@ -17830,7 +17882,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -19058,7 +19110,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="36" customHeight="1">
+    <row r="33" spans="1:11" ht="36" customHeight="1">
       <c r="A33" s="17" t="s">
         <v>73</v>
       </c>
@@ -19095,103 +19147,115 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="36" customHeight="1">
-      <c r="A34" s="17"/>
+    <row r="34" spans="1:11" ht="36" customHeight="1">
+      <c r="A34" s="17" t="s">
+        <v>75</v>
+      </c>
       <c r="B34" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@Paluska2000</v>
       </c>
       <c r="C34" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@Paluska2000]</v>
       </c>
       <c r="D34" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2000</v>
       </c>
       <c r="E34" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Paluska,  Scott A. and Schwenk,  Thomas L.</v>
       </c>
       <c r="F34" s="12" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>Physical Activity and Mental Health: Current Concepts</v>
       </c>
       <c r="G34" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H34" s="15" t="str">
+        <v>https://doi.org/10.2165/00007256-200029030-00003</v>
+      </c>
+      <c r="H34" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45592.857124652779</v>
       </c>
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" ht="36" customHeight="1">
-      <c r="A35" s="17"/>
+      <c r="J34" s="30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="36" customHeight="1">
+      <c r="A35" s="17" t="s">
+        <v>77</v>
+      </c>
       <c r="B35" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@Mikkelsen2017</v>
       </c>
       <c r="C35" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@Mikkelsen2017]</v>
       </c>
       <c r="D35" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2017</v>
       </c>
       <c r="E35" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Mikkelsen,  Kathleen and Stojanovska,  Lily and Polenakovic,  Momir and Bosevski,  Marijan and Apostolopoulos,  Vasso</v>
       </c>
       <c r="F35" s="12" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>Exercise and mental health</v>
       </c>
       <c r="G35" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H35" s="15" t="str">
+        <v>https://doi.org/10.1016/j.maturitas.2017.09.003</v>
+      </c>
+      <c r="H35" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45592.857473842596</v>
       </c>
       <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" ht="36" customHeight="1">
-      <c r="A36" s="17"/>
+      <c r="K35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="36" customHeight="1">
+      <c r="A36" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="B36" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@Carter2016</v>
       </c>
       <c r="C36" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@Carter2016]</v>
       </c>
       <c r="D36" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2016</v>
       </c>
       <c r="E36" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Carter,  Tim and Morres,  Ioannis D. and Meade,  Oonagh and Callaghan,  Patrick</v>
       </c>
       <c r="F36" s="12" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>The Effect of Exercise on Depressive Symptoms in Adolescents: A Systematic Review and Meta-Analysis</v>
       </c>
       <c r="G36" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H36" s="15" t="str">
+        <v>https://doi.org/10.1016/j.jaac.2016.04.016</v>
+      </c>
+      <c r="H36" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45592.861726620373</v>
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:10" ht="36" customHeight="1">
+    <row r="37" spans="1:11" ht="36" customHeight="1">
       <c r="A37" s="17"/>
       <c r="B37" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19223,7 +19287,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:10" ht="36" customHeight="1">
+    <row r="38" spans="1:11" ht="36" customHeight="1">
       <c r="A38" s="17"/>
       <c r="B38" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19255,7 +19319,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:10" ht="36" customHeight="1">
+    <row r="39" spans="1:11" ht="36" customHeight="1">
       <c r="A39" s="17"/>
       <c r="B39" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19287,7 +19351,7 @@
       </c>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:10" ht="36" customHeight="1">
+    <row r="40" spans="1:11" ht="36" customHeight="1">
       <c r="A40" s="17"/>
       <c r="B40" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19319,7 +19383,7 @@
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:10" ht="36" customHeight="1">
+    <row r="41" spans="1:11" ht="36" customHeight="1">
       <c r="A41" s="17"/>
       <c r="B41" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19351,7 +19415,7 @@
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:10" ht="36" customHeight="1">
+    <row r="42" spans="1:11" ht="36" customHeight="1">
       <c r="A42" s="17"/>
       <c r="B42" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19383,7 +19447,7 @@
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:10" ht="36" customHeight="1">
+    <row r="43" spans="1:11" ht="36" customHeight="1">
       <c r="A43" s="17"/>
       <c r="B43" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19415,7 +19479,7 @@
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:10" ht="36" customHeight="1">
+    <row r="44" spans="1:11" ht="36" customHeight="1">
       <c r="A44" s="17"/>
       <c r="B44" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19447,7 +19511,7 @@
       </c>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:10" ht="36" customHeight="1">
+    <row r="45" spans="1:11" ht="36" customHeight="1">
       <c r="A45" s="17"/>
       <c r="B45" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19479,7 +19543,7 @@
       </c>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:10" ht="36" customHeight="1">
+    <row r="46" spans="1:11" ht="36" customHeight="1">
       <c r="A46" s="17"/>
       <c r="B46" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19511,7 +19575,7 @@
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:10" ht="36" customHeight="1">
+    <row r="47" spans="1:11" ht="36" customHeight="1">
       <c r="A47" s="17"/>
       <c r="B47" s="13" t="str">
         <f t="shared" si="0"/>
@@ -19543,7 +19607,7 @@
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:10" ht="36" customHeight="1">
+    <row r="48" spans="1:11" ht="36" customHeight="1">
       <c r="A48" s="17"/>
       <c r="B48" s="13" t="str">
         <f t="shared" si="0"/>
@@ -34153,11 +34217,12 @@
     <hyperlink ref="J31" r:id="rId7" xr:uid="{678649AF-5D7E-4ACA-8A7F-E9D34255A849}"/>
     <hyperlink ref="J32" r:id="rId8" xr:uid="{1DFF1E7D-B6CF-46E4-8DDC-8041FD898A3E}"/>
     <hyperlink ref="J33" r:id="rId9" xr:uid="{00B217BF-927C-4C6A-8DC3-DA0FD6972FFD}"/>
+    <hyperlink ref="J34" r:id="rId10" xr:uid="{6475CF80-FCA4-4093-BD94-7CDEAE4F05EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId10"/>
-  <legacyDrawing r:id="rId11"/>
+  <drawing r:id="rId11"/>
+  <legacyDrawing r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -34173,15 +34238,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -34206,176 +34271,176 @@
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="72.75" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="32" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="23" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="180" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="210" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="255" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="255" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="285" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="285" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105" customHeight="1">
       <c r="A19" s="25" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120" customHeight="1">
       <c r="A20" s="25" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135" customHeight="1">
       <c r="A21" s="25" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I wrote a little more in the introduction and added the info on the Relapse prevention model from the exposé
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit mit bindr/Markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17E49C7D-EDDC-47D4-BF17-AEBBFCAD6101}"/>
+  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80E467ED-8FEA-451D-9733-87B5B7D7F2D5}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="127">
   <si>
     <t>@article{example2024,   title = {A Reference Example},   journal = {Journal of Examples},   publisher = {Example Press},   author = {Doe, Jane},   year = {2024},   month = aug,   pages = {185–209} }</t>
   </si>
@@ -680,6 +680,22 @@
   year = {2016},
   month = jul,
   pages = {580–590}
+}</t>
+  </si>
+  <si>
+    <t>@article{Gillison2009,
+  title = {The effects of exercise interventions on quality of life in clinical and healthy populations; a meta-analysis},
+  volume = {68},
+  ISSN = {0277-9536},
+  url = {http://dx.doi.org/10.1016/j.socscimed.2009.02.028},
+  DOI = {10.1016/j.socscimed.2009.02.028},
+  number = {9},
+  journal = {Social Science &amp;amp; Medicine},
+  publisher = {Elsevier BV},
+  author = {Gillison,  Fiona Bridget and Skevington,  Suzanne M. and Sato,  Ayana and Standage,  Martyn and Evangelidou,  Stella},
+  year = {2009},
+  month = may,
+  pages = {1700–1710}
 }</t>
   </si>
   <si>
@@ -17881,8 +17897,8 @@
   <dimension ref="A1:R505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -19256,34 +19272,36 @@
       <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:11" ht="36" customHeight="1">
-      <c r="A37" s="17"/>
+      <c r="A37" s="17" t="s">
+        <v>80</v>
+      </c>
       <c r="B37" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@Gillison2009</v>
       </c>
       <c r="C37" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@Gillison2009]</v>
       </c>
       <c r="D37" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2009</v>
       </c>
       <c r="E37" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Gillison,  Fiona Bridget and Skevington,  Suzanne M. and Sato,  Ayana and Standage,  Martyn and Evangelidou,  Stella</v>
       </c>
       <c r="F37" s="12" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>The effects of exercise interventions on quality of life in clinical and healthy populations; a meta-analysis</v>
       </c>
       <c r="G37" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H37" s="15" t="str">
+        <v>https://doi.org/10.1016/j.socscimed.2009.02.028</v>
+      </c>
+      <c r="H37" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45593.794906365743</v>
       </c>
       <c r="I37" s="1"/>
     </row>
@@ -34238,15 +34256,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -34271,176 +34289,176 @@
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="72.75" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="32" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="180" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="210" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="255" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="255" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="285" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="285" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105" customHeight="1">
       <c r="A19" s="25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120" customHeight="1">
       <c r="A20" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135" customHeight="1">
       <c r="A21" s="25" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1 corrected errors in references 2 added a demographics table and added the necessary packages 3 integrated both tables in apa format.
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit mit bindr/Markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="119" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80E467ED-8FEA-451D-9733-87B5B7D7F2D5}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5056FFA-04A0-4551-BA50-6F9492B5493B}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -266,7 +266,7 @@
   url = {http://dx.doi.org/10.1080/08870446.2015.1022547},
   DOI = {10.1080/08870446.2015.1022547},
   number = {9},
-  journal = {Psychology &amp;amp; Health},
+  journal = {Psychology &amp;; Health},
   publisher = {Informa UK Limited},
   author = {Mack,  Diane E. and Kouali,  Despina and Gilchrist,  Jenna D. and Sabiston,  Catherine M.},
   year = {2015},
@@ -427,7 +427,7 @@
   url = {http://dx.doi.org/10.1080/08870446.2021.1981900},
   DOI = {10.1080/08870446.2021.1981900},
   number = {5},
-  journal = {Psychology &amp;amp; Health},
+  journal = {Psychology &amp;; Health},
   publisher = {Informa UK Limited},
   author = {Roordink,  Eline M. and Steenhuis,  Ingrid H. M. and Kroeze,  Willemieke and Schoonmade,  Linda J. and Sniehotta,  Falko F. and van Stralen,  Maartje M.},
   year = {2021},
@@ -495,8 +495,8 @@
   year = {2020},
   publisher = {John Wiley \&amp; Sons, Inc.},
   address = {Hoboken, NJ},
-  pages = {xx--xx},
-  doi = {https://doi.org/10.1002/9781119568124.ch37}
+  pages = {773–794},
+  doi = {doi.org/10.1002/9781119568124.ch37}
 }</t>
   </si>
   <si>
@@ -527,7 +527,7 @@
   <si>
     <t>@incollection{Buckworth2007,
   author = {Buckworth, Janet and Dishman, Rodney K.},
-  title = {Exercise Adherence},
+  title = {Exercise adherence},
   booktitle = {Handbook of Sport Psychology},
   editor = {Tenenbaum, Gershon and Eklund, Robert C.},
   year = {2007},
@@ -674,7 +674,7 @@
   url = {http://dx.doi.org/10.1016/j.jaac.2016.04.016},
   DOI = {10.1016/j.jaac.2016.04.016},
   number = {7},
-  journal = {Journal of the American Academy of Child &amp;amp; Adolescent Psychiatry},
+  journal = {Journal of the American Academy of Child &amp;; Adolescent Psychiatry},
   publisher = {Elsevier BV},
   author = {Carter,  Tim and Morres,  Ioannis D. and Meade,  Oonagh and Callaghan,  Patrick},
   year = {2016},
@@ -690,7 +690,7 @@
   url = {http://dx.doi.org/10.1016/j.socscimed.2009.02.028},
   DOI = {10.1016/j.socscimed.2009.02.028},
   number = {9},
-  journal = {Social Science &amp;amp; Medicine},
+  journal = {Social Science &amp;; Medicine},
   publisher = {Elsevier BV},
   author = {Gillison,  Fiona Bridget and Skevington,  Suzanne M. and Sato,  Ayana and Standage,  Martyn and Evangelidou,  Stella},
   year = {2009},
@@ -17897,8 +17897,8 @@
   <dimension ref="A1:R505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -18891,7 +18891,7 @@
       </c>
       <c r="G26" s="14" t="str">
         <f t="shared" si="4"/>
-        <v>https://doi.org/https://doi.org/10.1002/9781119568124.ch37</v>
+        <v>https://doi.org/doi.org/10.1002/9781119568124.ch37</v>
       </c>
       <c r="H26" s="15">
         <f t="shared" ca="1" si="5"/>
@@ -18964,7 +18964,7 @@
       </c>
       <c r="F28" s="12" t="str">
         <f t="shared" ref="F28:F29" si="12">IFERROR(IF(ISERROR(FIND("title =",A28)),"",MID(A28,FIND("title =",A28)+9,FIND("},",A28,FIND("title =",A28))-FIND("title =",A28)-9)),"")</f>
-        <v>Exercise Adherence</v>
+        <v>Exercise adherence</v>
       </c>
       <c r="G28" s="14" t="str">
         <f t="shared" ref="G28:G29" si="13">IFERROR("https://doi.org/" &amp; MID(A28, SEARCH("doi = {", A28) + 7, FIND("}", A28, SEARCH("doi = {", A28)) - SEARCH("doi = {", A28) - 7),"")</f>

</xml_diff>

<commit_message>
Finished draft of all instruments. Updatet the links in the excel-reference-file to restrict access.
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit mit bindr/Markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{921B609B-1804-47B9-AF93-10A0E28CF695}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CF8420D-5ADB-482F-A4C2-AA285B63E302}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
   <si>
     <t>@article{example2024,   title = {A Reference Example},   journal = {Journal of Examples},   publisher = {Example Press},   author = {Doe, Jane},   year = {2024},   month = aug,   pages = {185–209} }</t>
   </si>
@@ -116,32 +116,16 @@
     <t>Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">@Inbook{Eckert2014,
-author = {Eckert, Katharina
-and Lange, Martin
-and Wagner, Petra},
-editor = {Becker, Simone},
-title = {Erfassung körperlicher Aktivität - Ein überblick über Anspruch und Realität einer validen Messung},
-bookTitle = {Aktiv und Gesund? Interdisziplinäre Perspektiven auf den Zusammenhang zwischen Sport und Gesundheit},
-year = {2014},
-publisher = {Springer Fachmedien Wiesbaden},
-address = {Wiesbaden},
-pages = {97--124},
-abstract = {Körperliche Aktivität ist in Prävention und Rehabilitation eine evidente Gesundheitsressource. Insgesamt weiß man aber noch zu wenig über das Dosis-Wirkungsgefüge hinsichtlich Art, Umfang und Intensität der körperlichen Aktivität auf verschiedene Gesundheitsparameter. Dies hängt u.a. damit zusammen, dass die akkurate Messung körperlicher Aktivität, trotz einer Vielzahl bestehender objektiver und subjektiver Erfassungsmethoden, nach wie vor unbefriedigend ausfällt.},
-isbn = {978-3-531-19063-1},
-doi = {10.1007/978-3-531-19063-1_5},
-url = {https://doi.org/10.1007/978-3-531-19063-1_5}
+    <t xml:space="preserve">@incollection{assembly2017resolution,
+  title = {{Resolution adopted by the General Assembly on 6 July 2017}},
+  author = {{United Nations General Assembly}},
+  booktitle = {Technical Report A/RES/71/313},
+  year = {2017}
 }
 </t>
   </si>
   <si>
-    <t>instruments</t>
-  </si>
-  <si>
-    <t>https://ennosgermancourse-my.sharepoint.com/:b:/g/personal/enno_winkler_spb-ew_de/EUJ3w2SonT9Ih2iG7LLOBlwBojuRYO6JTa0wkDmaB0gXQg?e=Qm5eNY</t>
-  </si>
-  <si>
-    <t>Messung körperlicher Aktivität, außerdem gutes Sammelwerk</t>
+    <t>intro</t>
   </si>
   <si>
     <t>@article{Foster2021,
@@ -160,6 +144,9 @@
 }</t>
   </si>
   <si>
+    <t>instruments</t>
+  </si>
+  <si>
     <t>@article{Peterson1982,
   title = {The attributional Style Questionnaire},
   volume = {6},
@@ -176,21 +163,7 @@
 }</t>
   </si>
   <si>
-    <t>@article{Tompuri2015,
-  title = {Metabolic equivalents of task are confounded by adiposity,  which disturbs objective measurement of physical activity},
-  volume = {6},
-  ISSN = {1664-042X},
-  url = {http://dx.doi.org/10.3389/fphys.2015.00226},
-  DOI = {10.3389/fphys.2015.00226},
-  journal = {Frontiers in Physiology},
-  publisher = {Frontiers Media SA},
-  author = {Tompuri,  Tuomo T.},
-  year = {2015},
-  month = aug 
-}</t>
-  </si>
-  <si>
-    <t>MET might not be ideal --&gt; Session RPE should be preferred</t>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/Attribution%20Questionnaire.pdf?csf=1&amp;web=1&amp;e=2zOMdl</t>
   </si>
   <si>
     <t>@article{Watson1988,
@@ -208,22 +181,6 @@
 }</t>
   </si>
   <si>
-    <t>@article{Foster2017,
-  title = {Monitoring Training Loads: The Past,  the Present,  and the Future},
-  volume = {12},
-  ISSN = {1555-0273},
-  url = {http://dx.doi.org/10.1123/IJSPP.2016-0388},
-  DOI = {10.1123/ijspp.2016-0388},
-  number = {s2},
-  journal = {International Journal of Sports Physiology and Performance},
-  publisher = {Human Kinetics},
-  author = {Foster,  Carl and Rodriguez-Marroyo,  Jose A. and de Koning,  Jos J.},
-  year = {2017},
-  month = apr,
-  pages = {S2--2--S2--8}
-}</t>
-  </si>
-  <si>
     <t>@misc{RKI_2022,
   author = {{Robert Koch-Institut}},
   title = {{Dashboard zu Gesundheit in Deutschland aktuell - GEDA 2019/2020}},
@@ -234,18 +191,6 @@
 }</t>
   </si>
   <si>
-    <t>intro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@incollection{assembly2017resolution,
-  title = {{Resolution adopted by the General Assembly on 6 July 2017}},
-  author = {{United Nations General Assembly}},
-  booktitle = {Technical Report A/RES/71/313},
-  year = {2017}
-}
-</t>
-  </si>
-  <si>
     <t>@book{WHO_2023,
   author = {{World Health Organization}},
   title = {Step Up! Tackling the Burden of Insufficient Physical Activity in Europe},
@@ -253,22 +198,6 @@
   publisher = {World Health Organization},
   url = {https://iris.who.int/handle/10665/366327}
 }</t>
-  </si>
-  <si>
-    <t>@book{hollmann2009sportmedizin,
-  author = {Hollmann, Wildor and Strüder, Heiko K.},
-  title = {Sportmedizin. Grundlagen für physische Aktivität, Training und Präventivmedizin},
-  edition = {5th},
-  publisher = {Schattauer},
-  year = {2009}
-}</t>
-  </si>
-  <si>
-    <t>overview</t>
-  </si>
-  <si>
-    <t>Definitinon - Physische Aktivität umfasst alle Tätigkeiten, die eine Steigerung des Energieumsatzes des 
-Körpers durch den Einsatz von Muskelkraft zur Folge haben</t>
   </si>
   <si>
     <t>@article{Amireault2013,
@@ -288,22 +217,6 @@
   </si>
   <si>
     <t>previous finding</t>
-  </si>
-  <si>
-    <t>@article{Roordink2021,
-  title = {Predictors of lapse and relapse in physical activity and dietary behaviour: a systematic search and review on prospective studies},
-  volume = {38},
-  ISSN = {1476-8321},
-  url = {http://dx.doi.org/10.1080/08870446.2021.1981900},
-  DOI = {10.1080/08870446.2021.1981900},
-  number = {5},
-  journal = {Psychology &amp;; Health},
-  publisher = {Informa UK Limited},
-  author = {Roordink,  Eline M. and Steenhuis,  Ingrid H. M. and Kroeze,  Willemieke and Schoonmade,  Linda J. and Sniehotta,  Falko F. and van Stralen,  Maartje M.},
-  year = {2021},
-  month = dec,
-  pages = {623–646}
-}</t>
   </si>
   <si>
     <t>@article{Gilchrist2018Pride,
@@ -419,7 +332,7 @@
 }</t>
   </si>
   <si>
-    <t>Exercise Slips in High-Risk Situations and Activity Patterns in Long-Term Exercisers.pdf</t>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/Exercise%20Slips%20in%20High-Risk%20Situations%20and%20Activity%20Patterns%20in%20Long-Term%20Exercisers.pdf?csf=1&amp;web=1&amp;e=geTkBC</t>
   </si>
   <si>
     <t xml:space="preserve">  @Article{lme4,
@@ -449,7 +362,81 @@
 }</t>
   </si>
   <si>
-    <t>British Journal of Addiction - December 1984 - Marlatt - Relapse Prevention Introduction and Overview of the Model.pdf</t>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/British%20Journal%20of%20Addiction%20-%20December%201984%20-%20Marlatt%20-%20Relapse%20Prevention%20Introduction%20and%20Overview%20of%20the%20Model.pdf?csf=1&amp;web=1&amp;e=1bgEat</t>
+  </si>
+  <si>
+    <t>@article{Tompuri2015,
+  title = {Metabolic equivalents of task are confounded by adiposity,  which disturbs objective measurement of physical activity},
+  volume = {6},
+  ISSN = {1664-042X},
+  url = {http://dx.doi.org/10.3389/fphys.2015.00226},
+  DOI = {10.3389/fphys.2015.00226},
+  journal = {Frontiers in Physiology},
+  publisher = {Frontiers Media SA},
+  author = {Tompuri,  Tuomo T.},
+  year = {2015},
+  month = aug 
+}</t>
+  </si>
+  <si>
+    <t>MET might not be ideal --&gt; Session RPE should be preferred</t>
+  </si>
+  <si>
+    <t>@book{hollmann2009sportmedizin,
+  author = {Hollmann, Wildor and Strüder, Heiko K.},
+  title = {Sportmedizin. Grundlagen für physische Aktivität, Training und Präventivmedizin},
+  edition = {5th},
+  publisher = {Schattauer},
+  year = {2009}
+}</t>
+  </si>
+  <si>
+    <t>overview</t>
+  </si>
+  <si>
+    <t>Definitinon - Physische Aktivität umfasst alle Tätigkeiten, die eine Steigerung des Energieumsatzes des 
+Körpers durch den Einsatz von Muskelkraft zur Folge haben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@Inbook{Eckert2014,
+author = {Eckert, Katharina
+and Lange, Martin
+and Wagner, Petra},
+editor = {Becker, Simone},
+title = {Erfassung körperlicher Aktivität - Ein überblick über Anspruch und Realität einer validen Messung},
+bookTitle = {Aktiv und Gesund? Interdisziplinäre Perspektiven auf den Zusammenhang zwischen Sport und Gesundheit},
+year = {2014},
+publisher = {Springer Fachmedien Wiesbaden},
+address = {Wiesbaden},
+pages = {97--124},
+abstract = {Körperliche Aktivität ist in Prävention und Rehabilitation eine evidente Gesundheitsressource. Insgesamt weiß man aber noch zu wenig über das Dosis-Wirkungsgefüge hinsichtlich Art, Umfang und Intensität der körperlichen Aktivität auf verschiedene Gesundheitsparameter. Dies hängt u.a. damit zusammen, dass die akkurate Messung körperlicher Aktivität, trotz einer Vielzahl bestehender objektiver und subjektiver Erfassungsmethoden, nach wie vor unbefriedigend ausfällt.},
+isbn = {978-3-531-19063-1},
+doi = {10.1007/978-3-531-19063-1_5},
+url = {https://doi.org/10.1007/978-3-531-19063-1_5}
+}
+</t>
+  </si>
+  <si>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/Aktiv%20und%20gesund.pdf?csf=1&amp;web=1&amp;e=cnifhs</t>
+  </si>
+  <si>
+    <t>Messung körperlicher Aktivität, außerdem gutes Sammelwerk</t>
+  </si>
+  <si>
+    <t>@article{Roordink2021,
+  title = {Predictors of lapse and relapse in physical activity and dietary behaviour: a systematic search and review on prospective studies},
+  volume = {38},
+  ISSN = {1476-8321},
+  url = {http://dx.doi.org/10.1080/08870446.2021.1981900},
+  DOI = {10.1080/08870446.2021.1981900},
+  number = {5},
+  journal = {Psychology &amp;; Health},
+  publisher = {Informa UK Limited},
+  author = {Roordink,  Eline M. and Steenhuis,  Ingrid H. M. and Kroeze,  Willemieke and Schoonmade,  Linda J. and Sniehotta,  Falko F. and van Stralen,  Maartje M.},
+  year = {2021},
+  month = dec,
+  pages = {623–646}
+}</t>
   </si>
   <si>
     <t>@article{Piggin2020,
@@ -466,7 +453,7 @@
 }</t>
   </si>
   <si>
-    <t>241023Piggin_Definition_PA.pdf</t>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/241023Piggin_Definition_PA.pdf?csf=1&amp;web=1&amp;e=InYJdt</t>
   </si>
   <si>
     <t>PA soll holistischer verstanden werden</t>
@@ -535,7 +522,7 @@
 }</t>
   </si>
   <si>
-    <t>https://ennosgermancourse-my.sharepoint.com/:b:/g/personal/enno_winkler_spb-ew_de/EZ-y0GL6TxxOrwdeWG1omaABUlSemHCzt7qm2t-Wvsaa4g?e=jrXqZS</t>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/Exercise%20Adherence.pdf?csf=1&amp;web=1&amp;e=tPkspJ</t>
   </si>
   <si>
     <t>und hat in der Regel das Ziel der Bewegungsförderung in einem gesundheitlichen Kontext [@Ainsworth2020].</t>
@@ -715,6 +702,22 @@
 }</t>
   </si>
   <si>
+    <t>@article{Foster2017,
+  title = {Monitoring Training Loads: The Past,  the Present,  and the Future},
+  volume = {12},
+  ISSN = {1555-0273},
+  url = {http://dx.doi.org/10.1123/IJSPP.2016-0388},
+  DOI = {10.1123/ijspp.2016-0388},
+  number = {s2},
+  journal = {International Journal of Sports Physiology and Performance},
+  publisher = {Human Kinetics},
+  author = {Foster,  Carl and Rodriguez-Marroyo,  Jose A. and de Koning,  Jos J.},
+  year = {2017},
+  month = apr,
+  pages = {S2--2--S2--8}
+}</t>
+  </si>
+  <si>
     <t>@article{Grant1998,
   author = {Grant, S. and Davidson, W. and Aitchison, T. and Wilson, J.},
   title = {A comparison of physiological responses and rating of perceived exertion between high-impact and low-impact aerobic dance sessions},
@@ -755,6 +758,65 @@
   author = {Day,  Meghan L. and McGuigan,  Michael R. and Brice,  Glenn and Foster,  Carl},
   year = {2004},
   pages = {353}
+}</t>
+  </si>
+  <si>
+    <t>@article{Crawford2004,
+  title = {The Positive and Negative Affect Schedule (PANAS): Construct validity,  measurement properties and normative data in a large non‐clinical sample},
+  volume = {43},
+  ISSN = {2044-8260},
+  url = {http://dx.doi.org/10.1348/0144665031752934},
+  DOI = {10.1348/0144665031752934},
+  number = {3},
+  journal = {British Journal of Clinical Psychology},
+  publisher = {Wiley},
+  author = {Crawford,  John R. and Henry,  Julie D.},
+  year = {2004},
+  month = sep,
+  pages = {245–265}
+}</t>
+  </si>
+  <si>
+    <t>@article{Corr1996,
+  title = {Structure and Validity of the Attributional Style Questionnaire: A Cross-Sample Comparison},
+  volume = {130},
+  ISSN = {1940-1019},
+  url = {http://dx.doi.org/10.1080/00223980.1996.9915038},
+  DOI = {10.1080/00223980.1996.9915038},
+  number = {6},
+  journal = {The Journal of Psychology},
+  publisher = {Informa UK Limited},
+  author = {Corr,  Philip J. and Gray,  Jeffrey A.},
+  year = {1996},
+  month = nov,
+  pages = {645–657}
+}</t>
+  </si>
+  <si>
+    <t>validierung ASQ</t>
+  </si>
+  <si>
+    <t>@book{winter1994manual,
+  title = {Manual for scoring motive imagery in running text:(Version 4.2)},
+  author = {Winter, David G},
+  year = {1994},
+  publisher = {Winter}
+}</t>
+  </si>
+  <si>
+    <t>@article{Sokolowski2000,
+  title = {Assessing Achievement,  Affiliation,  and Power Motives All at Once: The Multi-Motive Grid (MMG)},
+  volume = {74},
+  ISSN = {1532-7752},
+  url = {http://dx.doi.org/10.1207/S15327752JPA740109},
+  DOI = {10.1207/s15327752jpa740109},
+  number = {1},
+  journal = {Journal of Personality Assessment},
+  publisher = {Informa UK Limited},
+  author = {Sokolowski,  Kurt and Schmalt,  Heinz-Dieter and Langens,  Thomas A. and Puca,  Rosa M.},
+  year = {2000},
+  month = feb,
+  pages = {126–145}
 }</t>
   </si>
   <si>
@@ -17956,8 +18018,8 @@
   <dimension ref="A1:R505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <pane ySplit="1" topLeftCell="F9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -18044,1365 +18106,1368 @@
       </c>
       <c r="B2" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A2, SEARCH("{", A2) + 1, SEARCH(",", A2) - SEARCH("{", A2) - 1), "")</f>
-        <v>@Eckert2014</v>
+        <v>@assembly2017resolution</v>
       </c>
       <c r="C2" s="10" t="str">
         <f>"[" &amp; B2 &amp; "]"</f>
-        <v>[@Eckert2014]</v>
+        <v>[@assembly2017resolution]</v>
       </c>
       <c r="D2" s="11" t="str">
         <f>IFERROR(MID(A2,SEARCH("year = {",A2)+8,4), "")</f>
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="E2" s="11" t="str">
         <f>IFERROR(MID(A2, SEARCH("author = {", A2) + 10, SEARCH("}", A2, SEARCH("author = {", A2)) - SEARCH("author = {", A2) - 10), "")</f>
+        <v>{United Nations General Assembly</v>
+      </c>
+      <c r="F2" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A2)),"",MID(A2,FIND("title =",A2)+9,FIND("}",A2,FIND("title =",A2))-FIND("title =",A2)-9)),"")</f>
+        <v>{Resolution adopted by the General Assembly on 6 July 2017</v>
+      </c>
+      <c r="G2" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A2, SEARCH("doi = {", A2) + 7, FIND("}", A2, SEARCH("doi = {", A2)) - SEARCH("doi = {", A2) - 7),"")</f>
+        <v/>
+      </c>
+      <c r="H2" s="15">
+        <f ca="1">IF(A2&lt;&gt;"",IF(H2&lt;&gt;"",H2,NOW()),"")</f>
+        <v>45438.99941921296</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="36" customHeight="1">
+      <c r="A3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A3, SEARCH("{", A3) + 1, SEARCH(",", A3) - SEARCH("{", A3) - 1), "")</f>
+        <v>@Foster2021</v>
+      </c>
+      <c r="C3" s="10" t="str">
+        <f>"[" &amp; B3 &amp; "]"</f>
+        <v>[@Foster2021]</v>
+      </c>
+      <c r="D3" s="11" t="str">
+        <f>IFERROR(MID(A3,SEARCH("year = {",A3)+8,4), "")</f>
+        <v>2021</v>
+      </c>
+      <c r="E3" s="11" t="str">
+        <f>IFERROR(MID(A3, SEARCH("author = {", A3) + 10, SEARCH("}", A3, SEARCH("author = {", A3)) - SEARCH("author = {", A3) - 10), "")</f>
+        <v>Foster,  Carl and Boullosa,  Daniel and McGuigan,  Michael and Fusco,  Andrea and Cortis,  Cristina and Arney,  Blaine E. and Orton,  Bo and Dodge,  Christopher and Jaime,  Salvador and Radtke,  Kim and van Erp,  Teun and de Koning,  Jos J. and Bok,  Daniel and Rodriguez-Marroyo,  Jose A. and Porcari,  John P.</v>
+      </c>
+      <c r="F3" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A3)),"",MID(A3,FIND("title =",A3)+9,FIND("},",A3,FIND("title =",A3))-FIND("title =",A3)-9)),"")</f>
+        <v>25 Years of Session Rating of Perceived Exertion: Historical Perspective and Development</v>
+      </c>
+      <c r="G3" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A3, SEARCH("doi = {", A3) + 7, FIND("}", A3, SEARCH("doi = {", A3)) - SEARCH("doi = {", A3) - 7),"")</f>
+        <v>https://doi.org/10.1123/ijspp.2020-0599</v>
+      </c>
+      <c r="H3" s="15">
+        <f ca="1">IF(A3&lt;&gt;"",IF(H3&lt;&gt;"",H3,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="36" customHeight="1">
+      <c r="A4" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A4, SEARCH("{", A4) + 1, SEARCH(",", A4) - SEARCH("{", A4) - 1), "")</f>
+        <v>@Peterson1982</v>
+      </c>
+      <c r="C4" s="10" t="str">
+        <f>"[" &amp; B4 &amp; "]"</f>
+        <v>[@Peterson1982]</v>
+      </c>
+      <c r="D4" s="11" t="str">
+        <f>IFERROR(MID(A4,SEARCH("year = {",A4)+8,4), "")</f>
+        <v>1982</v>
+      </c>
+      <c r="E4" s="11" t="str">
+        <f>IFERROR(MID(A4, SEARCH("author = {", A4) + 10, SEARCH("}", A4, SEARCH("author = {", A4)) - SEARCH("author = {", A4) - 10), "")</f>
+        <v>Peterson,  Christopher and Semmel,  Amy and von Baeyer,  Carl and Abramson,  Lyn Y. and Metalsky,  Gerald I. and Seligman,  Martin E. P.</v>
+      </c>
+      <c r="F4" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A4)),"",MID(A4,FIND("title =",A4)+9,FIND("},",A4,FIND("title =",A4))-FIND("title =",A4)-9)),"")</f>
+        <v>The attributional Style Questionnaire</v>
+      </c>
+      <c r="G4" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A4, SEARCH("doi = {", A4) + 7, FIND("}", A4, SEARCH("doi = {", A4)) - SEARCH("doi = {", A4) - 7),"")</f>
+        <v>https://doi.org/10.1007/bf01173577</v>
+      </c>
+      <c r="H4" s="15">
+        <f ca="1">IF(A4&lt;&gt;"",IF(H4&lt;&gt;"",H4,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="36" customHeight="1">
+      <c r="A5" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A5, SEARCH("{", A5) + 1, SEARCH(",", A5) - SEARCH("{", A5) - 1), "")</f>
+        <v>@Watson1988</v>
+      </c>
+      <c r="C5" s="10" t="str">
+        <f>"[" &amp; B5 &amp; "]"</f>
+        <v>[@Watson1988]</v>
+      </c>
+      <c r="D5" s="11" t="str">
+        <f>IFERROR(MID(A5,SEARCH("year = {",A5)+8,4), "")</f>
+        <v>1988</v>
+      </c>
+      <c r="E5" s="11" t="str">
+        <f>IFERROR(MID(A5, SEARCH("author = {", A5) + 10, SEARCH("}", A5, SEARCH("author = {", A5)) - SEARCH("author = {", A5) - 10), "")</f>
+        <v>Watson,  David and Clark,  Lee Anna and Tellegen,  Auke</v>
+      </c>
+      <c r="F5" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A5)),"",MID(A5,FIND("title =",A5)+9,FIND("},",A5,FIND("title =",A5))-FIND("title =",A5)-9)),"")</f>
+        <v>Development and validation of brief measures of positive and negative affect: The PANAS scales.</v>
+      </c>
+      <c r="G5" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A5, SEARCH("doi = {", A5) + 7, FIND("}", A5, SEARCH("doi = {", A5)) - SEARCH("doi = {", A5) - 7),"")</f>
+        <v>https://doi.org/10.1037/0022-3514.54.6.1063</v>
+      </c>
+      <c r="H5" s="15">
+        <f ca="1">IF(A5&lt;&gt;"",IF(H5&lt;&gt;"",H5,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="36" customHeight="1">
+      <c r="A6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A6, SEARCH("{", A6) + 1, SEARCH(",", A6) - SEARCH("{", A6) - 1), "")</f>
+        <v>@RKI_2022</v>
+      </c>
+      <c r="C6" s="10" t="str">
+        <f>"[" &amp; B6 &amp; "]"</f>
+        <v>[@RKI_2022]</v>
+      </c>
+      <c r="D6" s="11" t="str">
+        <f>IFERROR(MID(A6,SEARCH("year = {",A6)+8,4), "")</f>
+        <v>2022</v>
+      </c>
+      <c r="E6" s="11" t="str">
+        <f>IFERROR(MID(A6, SEARCH("author = {", A6) + 10, SEARCH("}", A6, SEARCH("author = {", A6)) - SEARCH("author = {", A6) - 10), "")</f>
+        <v>{Robert Koch-Institut</v>
+      </c>
+      <c r="F6" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A6)),"",MID(A6,FIND("title =",A6)+9,FIND("}",A6,FIND("title =",A6))-FIND("title =",A6)-9)),"")</f>
+        <v>{Dashboard zu Gesundheit in Deutschland aktuell - GEDA 2019/2020</v>
+      </c>
+      <c r="G6" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A6, SEARCH("doi = {", A6) + 7, FIND("}", A6, SEARCH("doi = {", A6)) - SEARCH("doi = {", A6) - 7),"")</f>
+        <v>https://doi.org/10.25646/9362</v>
+      </c>
+      <c r="H6" s="15">
+        <f ca="1">IF(A6&lt;&gt;"",IF(H6&lt;&gt;"",H6,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="36" customHeight="1">
+      <c r="A7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A7, SEARCH("{", A7) + 1, SEARCH(",", A7) - SEARCH("{", A7) - 1), "")</f>
+        <v>@WHO_2023</v>
+      </c>
+      <c r="C7" s="10" t="str">
+        <f>"[" &amp; B7 &amp; "]"</f>
+        <v>[@WHO_2023]</v>
+      </c>
+      <c r="D7" s="11" t="str">
+        <f>IFERROR(MID(A7,SEARCH("year = {",A7)+8,4), "")</f>
+        <v>2023</v>
+      </c>
+      <c r="E7" s="11" t="str">
+        <f>IFERROR(MID(A7, SEARCH("author = {", A7) + 10, SEARCH("}", A7, SEARCH("author = {", A7)) - SEARCH("author = {", A7) - 10), "")</f>
+        <v>{World Health Organization</v>
+      </c>
+      <c r="F7" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A7)),"",MID(A7,FIND("title =",A7)+9,FIND("}",A7,FIND("title =",A7))-FIND("title =",A7)-9)),"")</f>
+        <v>Step Up! Tackling the Burden of Insufficient Physical Activity in Europe</v>
+      </c>
+      <c r="G7" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A7, SEARCH("doi = {", A7) + 7, FIND("}", A7, SEARCH("doi = {", A7)) - SEARCH("doi = {", A7) - 7),"")</f>
+        <v/>
+      </c>
+      <c r="H7" s="15">
+        <f ca="1">IF(A7&lt;&gt;"",IF(H7&lt;&gt;"",H7,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="36" customHeight="1">
+      <c r="A8" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A8, SEARCH("{", A8) + 1, SEARCH(",", A8) - SEARCH("{", A8) - 1), "")</f>
+        <v>@Amireault2013</v>
+      </c>
+      <c r="C8" s="10" t="str">
+        <f>"[" &amp; B8 &amp; "]"</f>
+        <v>[@Amireault2013]</v>
+      </c>
+      <c r="D8" s="11" t="str">
+        <f>IFERROR(MID(A8,SEARCH("year = {",A8)+8,4), "")</f>
+        <v>2013</v>
+      </c>
+      <c r="E8" s="11" t="str">
+        <f>IFERROR(MID(A8, SEARCH("author = {", A8) + 10, SEARCH("}", A8, SEARCH("author = {", A8)) - SEARCH("author = {", A8) - 10), "")</f>
+        <v>Amireault,  Steve and Godin,  Gaston and Vézina-Im,  Lydi-Anne</v>
+      </c>
+      <c r="F8" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A8)),"",MID(A8,FIND("title =",A8)+9,FIND("}",A8,FIND("title =",A8))-FIND("title =",A8)-9)),"")</f>
+        <v>Determinants of physical activity maintenance: a systematic review and meta-analyses</v>
+      </c>
+      <c r="G8" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A8, SEARCH("doi = {", A8) + 7, FIND("}", A8, SEARCH("doi = {", A8)) - SEARCH("doi = {", A8) - 7),"")</f>
+        <v>https://doi.org/10.1080/17437199.2012.701060</v>
+      </c>
+      <c r="H8" s="15">
+        <f ca="1">IF(A8&lt;&gt;"",IF(H8&lt;&gt;"",H8,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="36" customHeight="1">
+      <c r="A9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A9, SEARCH("{", A9) + 1, SEARCH(",", A9) - SEARCH("{", A9) - 1), "")</f>
+        <v>@Gilchrist2018Pride</v>
+      </c>
+      <c r="C9" s="10" t="str">
+        <f>"[" &amp; B9 &amp; "]"</f>
+        <v>[@Gilchrist2018Pride]</v>
+      </c>
+      <c r="D9" s="11" t="str">
+        <f>IFERROR(MID(A9,SEARCH("year = {",A9)+8,4), "")</f>
+        <v>2018</v>
+      </c>
+      <c r="E9" s="11" t="str">
+        <f>IFERROR(MID(A9, SEARCH("author = {", A9) + 10, SEARCH("}", A9, SEARCH("author = {", A9)) - SEARCH("author = {", A9) - 10), "")</f>
+        <v>Gilchrist,  Jenna D. and Sabiston,  Catherine M. and Conroy,  David E. and Atkinson,  Michael</v>
+      </c>
+      <c r="F9" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A9)),"",MID(A9,FIND("title =",A9)+9,FIND("},",A9,FIND("title =",A9))-FIND("title =",A9)-9)),"")</f>
+        <v>Authentic pride regulates runners’ training progress</v>
+      </c>
+      <c r="G9" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A9, SEARCH("doi = {", A9) + 7, FIND("}", A9, SEARCH("doi = {", A9)) - SEARCH("doi = {", A9) - 7),"")</f>
+        <v>https://doi.org/10.1016/j.psychsport.2018.05.007</v>
+      </c>
+      <c r="H9" s="15">
+        <f ca="1">IF(A9&lt;&gt;"",IF(H9&lt;&gt;"",H9,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="36" customHeight="1">
+      <c r="A10" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A10, SEARCH("{", A10) + 1, SEARCH(",", A10) - SEARCH("{", A10) - 1), "")</f>
+        <v>@Gilchrist2018Grit</v>
+      </c>
+      <c r="C10" s="10" t="str">
+        <f>"[" &amp; B10 &amp; "]"</f>
+        <v>[@Gilchrist2018Grit]</v>
+      </c>
+      <c r="D10" s="11" t="str">
+        <f>IFERROR(MID(A10,SEARCH("year = {",A10)+8,4), "")</f>
+        <v>2018</v>
+      </c>
+      <c r="E10" s="11" t="str">
+        <f>IFERROR(MID(A10, SEARCH("author = {", A10) + 10, SEARCH("}", A10, SEARCH("author = {", A10)) - SEARCH("author = {", A10) - 10), "")</f>
+        <v>Gilchrist, Jenna D. and Fong, Angela J. and Herbison, Jordan D. and Sabiston, Catherine M.</v>
+      </c>
+      <c r="F10" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A10)),"",MID(A10,FIND("title =",A10)+9,FIND("},",A10,FIND("title =",A10))-FIND("title =",A10)-9)),"")</f>
+        <v>Feelings of pride are associated with grit in student-athletes and recreational runners</v>
+      </c>
+      <c r="G10" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A10, SEARCH("doi = {", A10) + 7, FIND("}", A10, SEARCH("doi = {", A10)) - SEARCH("doi = {", A10) - 7),"")</f>
+        <v>https://doi.org/10.1016/J.PSYCHSPORT.2017.12.009</v>
+      </c>
+      <c r="H10" s="15">
+        <f ca="1">IF(A10&lt;&gt;"",IF(H10&lt;&gt;"",H10,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="60" customHeight="1">
+      <c r="A11" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A11, SEARCH("{", A11) + 1, SEARCH(",", A11) - SEARCH("{", A11) - 1), "")</f>
+        <v>@Mack2015</v>
+      </c>
+      <c r="C11" s="10" t="str">
+        <f>"[" &amp; B11 &amp; "]"</f>
+        <v>[@Mack2015]</v>
+      </c>
+      <c r="D11" s="11" t="str">
+        <f>IFERROR(MID(A11,SEARCH("year = {",A11)+8,4), "")</f>
+        <v>2015</v>
+      </c>
+      <c r="E11" s="11" t="str">
+        <f>IFERROR(MID(A11, SEARCH("author = {", A11) + 10, SEARCH("}", A11, SEARCH("author = {", A11)) - SEARCH("author = {", A11) - 10), "")</f>
+        <v>Mack,  Diane E. and Kouali,  Despina and Gilchrist,  Jenna D. and Sabiston,  Catherine M.</v>
+      </c>
+      <c r="F11" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A11)),"",MID(A11,FIND("title =",A11)+9,FIND("}",A11,FIND("title =",A11))-FIND("title =",A11)-9)),"")</f>
+        <v>Pride and physical activity: Behavioural regulations as a motivational mechanism?</v>
+      </c>
+      <c r="G11" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A11, SEARCH("doi = {", A11) + 7, FIND("}", A11, SEARCH("doi = {", A11)) - SEARCH("doi = {", A11) - 7),"")</f>
+        <v>https://doi.org/10.1080/08870446.2015.1022547</v>
+      </c>
+      <c r="H11" s="15">
+        <f ca="1">IF(A11&lt;&gt;"",IF(H11&lt;&gt;"",H11,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="36" customHeight="1">
+      <c r="A12" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A12, SEARCH("{", A12) + 1, SEARCH(",", A12) - SEARCH("{", A12) - 1), "")</f>
+        <v>@Tracy2007</v>
+      </c>
+      <c r="C12" s="10" t="str">
+        <f>"[" &amp; B12 &amp; "]"</f>
+        <v>[@Tracy2007]</v>
+      </c>
+      <c r="D12" s="11" t="str">
+        <f>IFERROR(MID(A12,SEARCH("year = {",A12)+8,4), "")</f>
+        <v>2007</v>
+      </c>
+      <c r="E12" s="11" t="str">
+        <f>IFERROR(MID(A12, SEARCH("author = {", A12) + 10, SEARCH("}", A12, SEARCH("author = {", A12)) - SEARCH("author = {", A12) - 10), "")</f>
+        <v>Tracy,  Jessica L. and Robins,  Richard W.</v>
+      </c>
+      <c r="F12" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A12)),"",MID(A12,FIND("title =",A12)+9,FIND("},",A12,FIND("title =",A12))-FIND("title =",A12)-9)),"")</f>
+        <v>Authentic And Hubristic Pride Scales</v>
+      </c>
+      <c r="G12" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A12, SEARCH("doi = {", A12) + 7, FIND("}", A12, SEARCH("doi = {", A12)) - SEARCH("doi = {", A12) - 7),"")</f>
+        <v>https://doi.org/10.1037/t06465-000</v>
+      </c>
+      <c r="H12" s="15">
+        <f ca="1">IF(A12&lt;&gt;"",IF(H12&lt;&gt;"",H12,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="36" customHeight="1">
+      <c r="A13" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A13, SEARCH("{", A13) + 1, SEARCH(",", A13) - SEARCH("{", A13) - 1), "")</f>
+        <v>@Marcus1997</v>
+      </c>
+      <c r="C13" s="10" t="str">
+        <f>"[" &amp; B13 &amp; "]"</f>
+        <v>[@Marcus1997]</v>
+      </c>
+      <c r="D13" s="11" t="str">
+        <f>IFERROR(MID(A13,SEARCH("year = {",A13)+8,4), "")</f>
+        <v>1997</v>
+      </c>
+      <c r="E13" s="11" t="str">
+        <f>IFERROR(MID(A13, SEARCH("author = {", A13) + 10, SEARCH("}", A13, SEARCH("author = {", A13)) - SEARCH("author = {", A13) - 10), "")</f>
+        <v>Marcus,  Bess H. and Bock,  Beth C. and Pinto,  Bernardine M.</v>
+      </c>
+      <c r="F13" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A13)),"",MID(A13,FIND("title =",A13)+9,FIND("}",A13,FIND("title =",A13))-FIND("title =",A13)-9)),"")</f>
+        <v>Initiation and Maintenance of Exercise Behavior</v>
+      </c>
+      <c r="G13" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A13, SEARCH("doi = {", A13) + 7, FIND("}", A13, SEARCH("doi = {", A13)) - SEARCH("doi = {", A13) - 7),"")</f>
+        <v>https://doi.org/10.1007/978-1-4899-1760-7_18</v>
+      </c>
+      <c r="H13" s="15">
+        <f ca="1">IF(A13&lt;&gt;"",IF(H13&lt;&gt;"",H13,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="36" customHeight="1">
+      <c r="A14" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A14, SEARCH("{", A14) + 1, SEARCH(",", A14) - SEARCH("{", A14) - 1), "")</f>
+        <v>@Marcus1993</v>
+      </c>
+      <c r="C14" s="10" t="str">
+        <f>"[" &amp; B14 &amp; "]"</f>
+        <v>[@Marcus1993]</v>
+      </c>
+      <c r="D14" s="11" t="str">
+        <f>IFERROR(MID(A14,SEARCH("year = {",A14)+8,4), "")</f>
+        <v>1993</v>
+      </c>
+      <c r="E14" s="11" t="str">
+        <f>IFERROR(MID(A14, SEARCH("author = {", A14) + 10, SEARCH("}", A14, SEARCH("author = {", A14)) - SEARCH("author = {", A14) - 10), "")</f>
+        <v>Marcus,  Bess H. and Stanton,  Annette L.</v>
+      </c>
+      <c r="F14" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A14)),"",MID(A14,FIND("title =",A14)+9,FIND("}",A14,FIND("title =",A14))-FIND("title =",A14)-9)),"")</f>
+        <v>Evaluation of Relapse Prevention and Reinforcement Interventions to Promote Exercise Adherence in Sedentary Females</v>
+      </c>
+      <c r="G14" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A14, SEARCH("doi = {", A14) + 7, FIND("}", A14, SEARCH("doi = {", A14)) - SEARCH("doi = {", A14) - 7),"")</f>
+        <v>https://doi.org/10.1080/02701367.1993.10607598</v>
+      </c>
+      <c r="H14" s="15">
+        <f ca="1">IF(A14&lt;&gt;"",IF(H14&lt;&gt;"",H14,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="36" customHeight="1">
+      <c r="A15" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A15, SEARCH("{", A15) + 1, SEARCH(",", A15) - SEARCH("{", A15) - 1), "")</f>
+        <v>@Martin1984</v>
+      </c>
+      <c r="C15" s="10" t="str">
+        <f>"[" &amp; B15 &amp; "]"</f>
+        <v>[@Martin1984]</v>
+      </c>
+      <c r="D15" s="11" t="str">
+        <f>IFERROR(MID(A15,SEARCH("year = {",A15)+8,4), "")</f>
+        <v>1984</v>
+      </c>
+      <c r="E15" s="11" t="str">
+        <f>IFERROR(MID(A15, SEARCH("author = {", A15) + 10, SEARCH("}", A15, SEARCH("author = {", A15)) - SEARCH("author = {", A15) - 10), "")</f>
+        <v>Martin,  John e. and Dubbert,  Patricia M. and Katell,  Alan D. and Thompson,  J. Kevin and Raczynski,  James R. and Lake,  Mary and Smith,  Patrick O. and Webster,  Jeffrey S. and Sikora,  Thomas and Cohen,  Randye E.</v>
+      </c>
+      <c r="F15" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A15)),"",MID(A15,FIND("title =",A15)+9,FIND("}",A15,FIND("title =",A15))-FIND("title =",A15)-9)),"")</f>
+        <v>Behavioral control of exercise in sedentary adults: Studies 1 through 6.</v>
+      </c>
+      <c r="G15" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A15, SEARCH("doi = {", A15) + 7, FIND("}", A15, SEARCH("doi = {", A15)) - SEARCH("doi = {", A15) - 7),"")</f>
+        <v>https://doi.org/10.1037/0022-006x.52.5.795</v>
+      </c>
+      <c r="H15" s="15">
+        <f ca="1">IF(A15&lt;&gt;"",IF(H15&lt;&gt;"",H15,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="36" customHeight="1">
+      <c r="A16" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A16, SEARCH("{", A16) + 1, SEARCH(",", A16) - SEARCH("{", A16) - 1), "")</f>
+        <v>@Stetson2005</v>
+      </c>
+      <c r="C16" s="10" t="str">
+        <f>"[" &amp; B16 &amp; "]"</f>
+        <v>[@Stetson2005]</v>
+      </c>
+      <c r="D16" s="11" t="str">
+        <f>IFERROR(MID(A16,SEARCH("year = {",A16)+8,4), "")</f>
+        <v>2005</v>
+      </c>
+      <c r="E16" s="11" t="str">
+        <f>IFERROR(MID(A16, SEARCH("author = {", A16) + 10, SEARCH("}", A16, SEARCH("author = {", A16)) - SEARCH("author = {", A16) - 10), "")</f>
+        <v>Stetson,  Barbara A. and Beacham,  Abbie O. and Frommelt,  Stephen J. and Boutelle,  Kerri N. and Cole,  Jonathan D. and Ziegler,  Craig H. and Looney,  Stephen W.</v>
+      </c>
+      <c r="F16" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A16)),"",MID(A16,FIND("title =",A16)+9,FIND("}",A16,FIND("title =",A16))-FIND("title =",A16)-9)),"")</f>
+        <v>Exercise slips in high-risk situations and activity patterns in long-term exercisers: An application of the relapse prevention model</v>
+      </c>
+      <c r="G16" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A16, SEARCH("doi = {", A16) + 7, FIND("}", A16, SEARCH("doi = {", A16)) - SEARCH("doi = {", A16) - 7),"")</f>
+        <v>https://doi.org/10.1207/s15324796abm3001_4</v>
+      </c>
+      <c r="H16" s="15">
+        <f ca="1">IF(A16&lt;&gt;"",IF(H16&lt;&gt;"",H16,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="36" customHeight="1">
+      <c r="A17" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A17, SEARCH("{", A17) + 1, SEARCH(",", A17) - SEARCH("{", A17) - 1), "")</f>
+        <v>@lme4</v>
+      </c>
+      <c r="C17" s="10" t="str">
+        <f>"[" &amp; B17 &amp; "]"</f>
+        <v>[@lme4]</v>
+      </c>
+      <c r="D17" s="11" t="str">
+        <f>IFERROR(MID(A17,SEARCH("year = {",A17)+8,4), "")</f>
+        <v>2015</v>
+      </c>
+      <c r="E17" s="11" t="str">
+        <f>IFERROR(MID(A17, SEARCH("author = {", A17) + 10, SEARCH("}", A17, SEARCH("author = {", A17)) - SEARCH("author = {", A17) - 10), "")</f>
+        <v>Douglas Bates and Martin Mächler and Ben Bolker and Steve Walker</v>
+      </c>
+      <c r="F17" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A17)),"",MID(A17,FIND("title =",A17)+9,FIND("},",A17,FIND("title =",A17))-FIND("title =",A17)-9)),"")</f>
+        <v>Fitting Linear Mixed-Effects Models Using {{lme4}}</v>
+      </c>
+      <c r="G17" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A17, SEARCH("doi = {", A17) + 7, FIND("}", A17, SEARCH("doi = {", A17)) - SEARCH("doi = {", A17) - 7),"")</f>
+        <v>https://doi.org/10.18637/jss.v067.i01</v>
+      </c>
+      <c r="H17" s="15">
+        <f ca="1">IF(A17&lt;&gt;"",IF(H17&lt;&gt;"",H17,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" ht="36" customHeight="1">
+      <c r="A18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A18, SEARCH("{", A18) + 1, SEARCH(",", A18) - SEARCH("{", A18) - 1), "")</f>
+        <v>@Marlatt1984</v>
+      </c>
+      <c r="C18" s="10" t="str">
+        <f>"[" &amp; B18 &amp; "]"</f>
+        <v>[@Marlatt1984]</v>
+      </c>
+      <c r="D18" s="11" t="str">
+        <f>IFERROR(MID(A18,SEARCH("year = {",A18)+8,4), "")</f>
+        <v>1984</v>
+      </c>
+      <c r="E18" s="11" t="str">
+        <f>IFERROR(MID(A18, SEARCH("author = {", A18) + 10, SEARCH("}", A18, SEARCH("author = {", A18)) - SEARCH("author = {", A18) - 10), "")</f>
+        <v>Marlatt,  G. Alan and George,  William H.</v>
+      </c>
+      <c r="F18" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A18)),"",MID(A18,FIND("title =",A18)+9,FIND("},",A18,FIND("title =",A18))-FIND("title =",A18)-9)),"")</f>
+        <v>Relapse Prevention: Introduction and Overview of the Model</v>
+      </c>
+      <c r="G18" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A18, SEARCH("doi = {", A18) + 7, FIND("}", A18, SEARCH("doi = {", A18)) - SEARCH("doi = {", A18) - 7),"")</f>
+        <v>https://doi.org/10.1111/j.1360-0443.1984.tb03867.x</v>
+      </c>
+      <c r="H18" s="15">
+        <f ca="1">IF(A18&lt;&gt;"",IF(H18&lt;&gt;"",H18,NOW()),"")</f>
+        <v>45580.951379513892</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="36" customHeight="1">
+      <c r="A19" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A19, SEARCH("{", A19) + 1, SEARCH(",", A19) - SEARCH("{", A19) - 1), "")</f>
+        <v>@Tompuri2015</v>
+      </c>
+      <c r="C19" s="10" t="str">
+        <f>"[" &amp; B19 &amp; "]"</f>
+        <v>[@Tompuri2015]</v>
+      </c>
+      <c r="D19" s="11" t="str">
+        <f>IFERROR(MID(A19,SEARCH("year = {",A19)+8,4), "")</f>
+        <v>2015</v>
+      </c>
+      <c r="E19" s="11" t="str">
+        <f>IFERROR(MID(A19, SEARCH("author = {", A19) + 10, SEARCH("}", A19, SEARCH("author = {", A19)) - SEARCH("author = {", A19) - 10), "")</f>
+        <v>Tompuri,  Tuomo T.</v>
+      </c>
+      <c r="F19" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A19)),"",MID(A19,FIND("title =",A19)+9,FIND("},",A19,FIND("title =",A19))-FIND("title =",A19)-9)),"")</f>
+        <v>Metabolic equivalents of task are confounded by adiposity,  which disturbs objective measurement of physical activity</v>
+      </c>
+      <c r="G19" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A19, SEARCH("doi = {", A19) + 7, FIND("}", A19, SEARCH("doi = {", A19)) - SEARCH("doi = {", A19) - 7),"")</f>
+        <v>https://doi.org/10.3389/fphys.2015.00226</v>
+      </c>
+      <c r="H19" s="15">
+        <f ca="1">IF(A19&lt;&gt;"",IF(H19&lt;&gt;"",H19,NOW()),"")</f>
+        <v>45581.499819907411</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="36" customHeight="1">
+      <c r="A20" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A20, SEARCH("{", A20) + 1, SEARCH(",", A20) - SEARCH("{", A20) - 1), "")</f>
+        <v>@hollmann2009sportmedizin</v>
+      </c>
+      <c r="C20" s="10" t="str">
+        <f>"[" &amp; B20 &amp; "]"</f>
+        <v>[@hollmann2009sportmedizin]</v>
+      </c>
+      <c r="D20" s="11" t="str">
+        <f>IFERROR(MID(A20,SEARCH("year = {",A20)+8,4), "")</f>
+        <v>2009</v>
+      </c>
+      <c r="E20" s="11" t="str">
+        <f>IFERROR(MID(A20, SEARCH("author = {", A20) + 10, SEARCH("}", A20, SEARCH("author = {", A20)) - SEARCH("author = {", A20) - 10), "")</f>
+        <v>Hollmann, Wildor and Strüder, Heiko K.</v>
+      </c>
+      <c r="F20" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A20)),"",MID(A20,FIND("title =",A20)+9,FIND("},",A20,FIND("title =",A20))-FIND("title =",A20)-9)),"")</f>
+        <v>Sportmedizin. Grundlagen für physische Aktivität, Training und Präventivmedizin</v>
+      </c>
+      <c r="G20" s="14" t="str">
+        <f>IFERROR("https://doi.org/" &amp; MID(A20, SEARCH("doi = {", A20) + 7, FIND("}", A20, SEARCH("doi = {", A20)) - SEARCH("doi = {", A20) - 7),"")</f>
+        <v/>
+      </c>
+      <c r="H20" s="15">
+        <f ca="1">IF(A20&lt;&gt;"",IF(H20&lt;&gt;"",H20,NOW()),"")</f>
+        <v>45581.507293287039</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="36" customHeight="1">
+      <c r="A21" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="13" t="str">
+        <f>IFERROR("@" &amp; MID(A21, SEARCH("{", A21) + 1, SEARCH(",", A21) - SEARCH("{", A21) - 1), "")</f>
+        <v>@Eckert2014</v>
+      </c>
+      <c r="C21" s="10" t="str">
+        <f>"[" &amp; B21 &amp; "]"</f>
+        <v>[@Eckert2014]</v>
+      </c>
+      <c r="D21" s="11" t="str">
+        <f>IFERROR(MID(A21,SEARCH("year = {",A21)+8,4), "")</f>
+        <v>2014</v>
+      </c>
+      <c r="E21" s="11" t="str">
+        <f>IFERROR(MID(A21, SEARCH("author = {", A21) + 10, SEARCH("}", A21, SEARCH("author = {", A21)) - SEARCH("author = {", A21) - 10), "")</f>
         <v>Eckert, Katharina
 and Lange, Martin
 and Wagner, Petra</v>
       </c>
-      <c r="F2" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A2)),"",MID(A2,FIND("title =",A2)+9,FIND("},",A2,FIND("title =",A2))-FIND("title =",A2)-9)),"")</f>
+      <c r="F21" s="12" t="str">
+        <f>IFERROR(IF(ISERROR(FIND("title =",A21)),"",MID(A21,FIND("title =",A21)+9,FIND("},",A21,FIND("title =",A21))-FIND("title =",A21)-9)),"")</f>
         <v>Erfassung körperlicher Aktivität - Ein überblick über Anspruch und Realität einer validen Messung</v>
-      </c>
-      <c r="G2" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A2, SEARCH("doi = {", A2) + 7, FIND("}", A2, SEARCH("doi = {", A2)) - SEARCH("doi = {", A2) - 7),"")</f>
-        <v>https://doi.org/10.1007/978-3-531-19063-1_5</v>
-      </c>
-      <c r="H2" s="15">
-        <f ca="1">IF(A2&lt;&gt;"",IF(H2&lt;&gt;"",H2,NOW()),"")</f>
-        <v>45581.517357060184</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="36" customHeight="1">
-      <c r="A3" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A3, SEARCH("{", A3) + 1, SEARCH(",", A3) - SEARCH("{", A3) - 1), "")</f>
-        <v>@Foster2021</v>
-      </c>
-      <c r="C3" s="10" t="str">
-        <f>"[" &amp; B3 &amp; "]"</f>
-        <v>[@Foster2021]</v>
-      </c>
-      <c r="D3" s="11" t="str">
-        <f>IFERROR(MID(A3,SEARCH("year = {",A3)+8,4), "")</f>
-        <v>2021</v>
-      </c>
-      <c r="E3" s="11" t="str">
-        <f>IFERROR(MID(A3, SEARCH("author = {", A3) + 10, SEARCH("}", A3, SEARCH("author = {", A3)) - SEARCH("author = {", A3) - 10), "")</f>
-        <v>Foster,  Carl and Boullosa,  Daniel and McGuigan,  Michael and Fusco,  Andrea and Cortis,  Cristina and Arney,  Blaine E. and Orton,  Bo and Dodge,  Christopher and Jaime,  Salvador and Radtke,  Kim and van Erp,  Teun and de Koning,  Jos J. and Bok,  Daniel and Rodriguez-Marroyo,  Jose A. and Porcari,  John P.</v>
-      </c>
-      <c r="F3" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A3)),"",MID(A3,FIND("title =",A3)+9,FIND("},",A3,FIND("title =",A3))-FIND("title =",A3)-9)),"")</f>
-        <v>25 Years of Session Rating of Perceived Exertion: Historical Perspective and Development</v>
-      </c>
-      <c r="G3" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A3, SEARCH("doi = {", A3) + 7, FIND("}", A3, SEARCH("doi = {", A3)) - SEARCH("doi = {", A3) - 7),"")</f>
-        <v>https://doi.org/10.1123/ijspp.2020-0599</v>
-      </c>
-      <c r="H3" s="15">
-        <f ca="1">IF(A3&lt;&gt;"",IF(H3&lt;&gt;"",H3,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="36" customHeight="1">
-      <c r="A4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A4, SEARCH("{", A4) + 1, SEARCH(",", A4) - SEARCH("{", A4) - 1), "")</f>
-        <v>@Peterson1982</v>
-      </c>
-      <c r="C4" s="10" t="str">
-        <f>"[" &amp; B4 &amp; "]"</f>
-        <v>[@Peterson1982]</v>
-      </c>
-      <c r="D4" s="11" t="str">
-        <f>IFERROR(MID(A4,SEARCH("year = {",A4)+8,4), "")</f>
-        <v>1982</v>
-      </c>
-      <c r="E4" s="11" t="str">
-        <f>IFERROR(MID(A4, SEARCH("author = {", A4) + 10, SEARCH("}", A4, SEARCH("author = {", A4)) - SEARCH("author = {", A4) - 10), "")</f>
-        <v>Peterson,  Christopher and Semmel,  Amy and von Baeyer,  Carl and Abramson,  Lyn Y. and Metalsky,  Gerald I. and Seligman,  Martin E. P.</v>
-      </c>
-      <c r="F4" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A4)),"",MID(A4,FIND("title =",A4)+9,FIND("},",A4,FIND("title =",A4))-FIND("title =",A4)-9)),"")</f>
-        <v>The attributional Style Questionnaire</v>
-      </c>
-      <c r="G4" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A4, SEARCH("doi = {", A4) + 7, FIND("}", A4, SEARCH("doi = {", A4)) - SEARCH("doi = {", A4) - 7),"")</f>
-        <v>https://doi.org/10.1007/bf01173577</v>
-      </c>
-      <c r="H4" s="15">
-        <f ca="1">IF(A4&lt;&gt;"",IF(H4&lt;&gt;"",H4,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="36" customHeight="1">
-      <c r="A5" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A5, SEARCH("{", A5) + 1, SEARCH(",", A5) - SEARCH("{", A5) - 1), "")</f>
-        <v>@Tompuri2015</v>
-      </c>
-      <c r="C5" s="10" t="str">
-        <f>"[" &amp; B5 &amp; "]"</f>
-        <v>[@Tompuri2015]</v>
-      </c>
-      <c r="D5" s="11" t="str">
-        <f>IFERROR(MID(A5,SEARCH("year = {",A5)+8,4), "")</f>
-        <v>2015</v>
-      </c>
-      <c r="E5" s="11" t="str">
-        <f>IFERROR(MID(A5, SEARCH("author = {", A5) + 10, SEARCH("}", A5, SEARCH("author = {", A5)) - SEARCH("author = {", A5) - 10), "")</f>
-        <v>Tompuri,  Tuomo T.</v>
-      </c>
-      <c r="F5" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A5)),"",MID(A5,FIND("title =",A5)+9,FIND("},",A5,FIND("title =",A5))-FIND("title =",A5)-9)),"")</f>
-        <v>Metabolic equivalents of task are confounded by adiposity,  which disturbs objective measurement of physical activity</v>
-      </c>
-      <c r="G5" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A5, SEARCH("doi = {", A5) + 7, FIND("}", A5, SEARCH("doi = {", A5)) - SEARCH("doi = {", A5) - 7),"")</f>
-        <v>https://doi.org/10.3389/fphys.2015.00226</v>
-      </c>
-      <c r="H5" s="15">
-        <f ca="1">IF(A5&lt;&gt;"",IF(H5&lt;&gt;"",H5,NOW()),"")</f>
-        <v>45581.499819907411</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="36" customHeight="1">
-      <c r="A6" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A6, SEARCH("{", A6) + 1, SEARCH(",", A6) - SEARCH("{", A6) - 1), "")</f>
-        <v>@Watson1988</v>
-      </c>
-      <c r="C6" s="10" t="str">
-        <f>"[" &amp; B6 &amp; "]"</f>
-        <v>[@Watson1988]</v>
-      </c>
-      <c r="D6" s="11" t="str">
-        <f>IFERROR(MID(A6,SEARCH("year = {",A6)+8,4), "")</f>
-        <v>1988</v>
-      </c>
-      <c r="E6" s="11" t="str">
-        <f>IFERROR(MID(A6, SEARCH("author = {", A6) + 10, SEARCH("}", A6, SEARCH("author = {", A6)) - SEARCH("author = {", A6) - 10), "")</f>
-        <v>Watson,  David and Clark,  Lee Anna and Tellegen,  Auke</v>
-      </c>
-      <c r="F6" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A6)),"",MID(A6,FIND("title =",A6)+9,FIND("},",A6,FIND("title =",A6))-FIND("title =",A6)-9)),"")</f>
-        <v>Development and validation of brief measures of positive and negative affect: The PANAS scales.</v>
-      </c>
-      <c r="G6" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A6, SEARCH("doi = {", A6) + 7, FIND("}", A6, SEARCH("doi = {", A6)) - SEARCH("doi = {", A6) - 7),"")</f>
-        <v>https://doi.org/10.1037/0022-3514.54.6.1063</v>
-      </c>
-      <c r="H6" s="15">
-        <f ca="1">IF(A6&lt;&gt;"",IF(H6&lt;&gt;"",H6,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="36" customHeight="1">
-      <c r="A7" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A7, SEARCH("{", A7) + 1, SEARCH(",", A7) - SEARCH("{", A7) - 1), "")</f>
-        <v>@Foster2017</v>
-      </c>
-      <c r="C7" s="10" t="str">
-        <f>"[" &amp; B7 &amp; "]"</f>
-        <v>[@Foster2017]</v>
-      </c>
-      <c r="D7" s="11" t="str">
-        <f>IFERROR(MID(A7,SEARCH("year = {",A7)+8,4), "")</f>
-        <v>2017</v>
-      </c>
-      <c r="E7" s="11" t="str">
-        <f>IFERROR(MID(A7, SEARCH("author = {", A7) + 10, SEARCH("}", A7, SEARCH("author = {", A7)) - SEARCH("author = {", A7) - 10), "")</f>
-        <v>Foster,  Carl and Rodriguez-Marroyo,  Jose A. and de Koning,  Jos J.</v>
-      </c>
-      <c r="F7" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A7)),"",MID(A7,FIND("title =",A7)+9,FIND("},",A7,FIND("title =",A7))-FIND("title =",A7)-9)),"")</f>
-        <v>Monitoring Training Loads: The Past,  the Present,  and the Future</v>
-      </c>
-      <c r="G7" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A7, SEARCH("doi = {", A7) + 7, FIND("}", A7, SEARCH("doi = {", A7)) - SEARCH("doi = {", A7) - 7),"")</f>
-        <v>https://doi.org/10.1123/ijspp.2016-0388</v>
-      </c>
-      <c r="H7" s="15">
-        <f ca="1">IF(A7&lt;&gt;"",IF(H7&lt;&gt;"",H7,NOW()),"")</f>
-        <v>45594.792853472223</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="36" customHeight="1">
-      <c r="A8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A8, SEARCH("{", A8) + 1, SEARCH(",", A8) - SEARCH("{", A8) - 1), "")</f>
-        <v>@RKI_2022</v>
-      </c>
-      <c r="C8" s="10" t="str">
-        <f>"[" &amp; B8 &amp; "]"</f>
-        <v>[@RKI_2022]</v>
-      </c>
-      <c r="D8" s="11" t="str">
-        <f>IFERROR(MID(A8,SEARCH("year = {",A8)+8,4), "")</f>
-        <v>2022</v>
-      </c>
-      <c r="E8" s="11" t="str">
-        <f>IFERROR(MID(A8, SEARCH("author = {", A8) + 10, SEARCH("}", A8, SEARCH("author = {", A8)) - SEARCH("author = {", A8) - 10), "")</f>
-        <v>{Robert Koch-Institut</v>
-      </c>
-      <c r="F8" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A8)),"",MID(A8,FIND("title =",A8)+9,FIND("}",A8,FIND("title =",A8))-FIND("title =",A8)-9)),"")</f>
-        <v>{Dashboard zu Gesundheit in Deutschland aktuell - GEDA 2019/2020</v>
-      </c>
-      <c r="G8" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A8, SEARCH("doi = {", A8) + 7, FIND("}", A8, SEARCH("doi = {", A8)) - SEARCH("doi = {", A8) - 7),"")</f>
-        <v>https://doi.org/10.25646/9362</v>
-      </c>
-      <c r="H8" s="15">
-        <f ca="1">IF(A8&lt;&gt;"",IF(H8&lt;&gt;"",H8,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="36" customHeight="1">
-      <c r="A9" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A9, SEARCH("{", A9) + 1, SEARCH(",", A9) - SEARCH("{", A9) - 1), "")</f>
-        <v>@assembly2017resolution</v>
-      </c>
-      <c r="C9" s="10" t="str">
-        <f>"[" &amp; B9 &amp; "]"</f>
-        <v>[@assembly2017resolution]</v>
-      </c>
-      <c r="D9" s="11" t="str">
-        <f>IFERROR(MID(A9,SEARCH("year = {",A9)+8,4), "")</f>
-        <v>2017</v>
-      </c>
-      <c r="E9" s="11" t="str">
-        <f>IFERROR(MID(A9, SEARCH("author = {", A9) + 10, SEARCH("}", A9, SEARCH("author = {", A9)) - SEARCH("author = {", A9) - 10), "")</f>
-        <v>{United Nations General Assembly</v>
-      </c>
-      <c r="F9" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A9)),"",MID(A9,FIND("title =",A9)+9,FIND("}",A9,FIND("title =",A9))-FIND("title =",A9)-9)),"")</f>
-        <v>{Resolution adopted by the General Assembly on 6 July 2017</v>
-      </c>
-      <c r="G9" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A9, SEARCH("doi = {", A9) + 7, FIND("}", A9, SEARCH("doi = {", A9)) - SEARCH("doi = {", A9) - 7),"")</f>
-        <v/>
-      </c>
-      <c r="H9" s="15">
-        <f ca="1">IF(A9&lt;&gt;"",IF(H9&lt;&gt;"",H9,NOW()),"")</f>
-        <v>45438.99941921296</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="36" customHeight="1">
-      <c r="A10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A10, SEARCH("{", A10) + 1, SEARCH(",", A10) - SEARCH("{", A10) - 1), "")</f>
-        <v>@WHO_2023</v>
-      </c>
-      <c r="C10" s="10" t="str">
-        <f>"[" &amp; B10 &amp; "]"</f>
-        <v>[@WHO_2023]</v>
-      </c>
-      <c r="D10" s="11" t="str">
-        <f>IFERROR(MID(A10,SEARCH("year = {",A10)+8,4), "")</f>
-        <v>2023</v>
-      </c>
-      <c r="E10" s="11" t="str">
-        <f>IFERROR(MID(A10, SEARCH("author = {", A10) + 10, SEARCH("}", A10, SEARCH("author = {", A10)) - SEARCH("author = {", A10) - 10), "")</f>
-        <v>{World Health Organization</v>
-      </c>
-      <c r="F10" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A10)),"",MID(A10,FIND("title =",A10)+9,FIND("}",A10,FIND("title =",A10))-FIND("title =",A10)-9)),"")</f>
-        <v>Step Up! Tackling the Burden of Insufficient Physical Activity in Europe</v>
-      </c>
-      <c r="G10" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A10, SEARCH("doi = {", A10) + 7, FIND("}", A10, SEARCH("doi = {", A10)) - SEARCH("doi = {", A10) - 7),"")</f>
-        <v/>
-      </c>
-      <c r="H10" s="15">
-        <f ca="1">IF(A10&lt;&gt;"",IF(H10&lt;&gt;"",H10,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="60" customHeight="1">
-      <c r="A11" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A11, SEARCH("{", A11) + 1, SEARCH(",", A11) - SEARCH("{", A11) - 1), "")</f>
-        <v>@hollmann2009sportmedizin</v>
-      </c>
-      <c r="C11" s="10" t="str">
-        <f>"[" &amp; B11 &amp; "]"</f>
-        <v>[@hollmann2009sportmedizin]</v>
-      </c>
-      <c r="D11" s="11" t="str">
-        <f>IFERROR(MID(A11,SEARCH("year = {",A11)+8,4), "")</f>
-        <v>2009</v>
-      </c>
-      <c r="E11" s="11" t="str">
-        <f>IFERROR(MID(A11, SEARCH("author = {", A11) + 10, SEARCH("}", A11, SEARCH("author = {", A11)) - SEARCH("author = {", A11) - 10), "")</f>
-        <v>Hollmann, Wildor and Strüder, Heiko K.</v>
-      </c>
-      <c r="F11" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A11)),"",MID(A11,FIND("title =",A11)+9,FIND("},",A11,FIND("title =",A11))-FIND("title =",A11)-9)),"")</f>
-        <v>Sportmedizin. Grundlagen für physische Aktivität, Training und Präventivmedizin</v>
-      </c>
-      <c r="G11" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A11, SEARCH("doi = {", A11) + 7, FIND("}", A11, SEARCH("doi = {", A11)) - SEARCH("doi = {", A11) - 7),"")</f>
-        <v/>
-      </c>
-      <c r="H11" s="15">
-        <f ca="1">IF(A11&lt;&gt;"",IF(H11&lt;&gt;"",H11,NOW()),"")</f>
-        <v>45581.507293287039</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" s="27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="36" customHeight="1">
-      <c r="A12" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A12, SEARCH("{", A12) + 1, SEARCH(",", A12) - SEARCH("{", A12) - 1), "")</f>
-        <v>@Amireault2013</v>
-      </c>
-      <c r="C12" s="10" t="str">
-        <f>"[" &amp; B12 &amp; "]"</f>
-        <v>[@Amireault2013]</v>
-      </c>
-      <c r="D12" s="11" t="str">
-        <f>IFERROR(MID(A12,SEARCH("year = {",A12)+8,4), "")</f>
-        <v>2013</v>
-      </c>
-      <c r="E12" s="11" t="str">
-        <f>IFERROR(MID(A12, SEARCH("author = {", A12) + 10, SEARCH("}", A12, SEARCH("author = {", A12)) - SEARCH("author = {", A12) - 10), "")</f>
-        <v>Amireault,  Steve and Godin,  Gaston and Vézina-Im,  Lydi-Anne</v>
-      </c>
-      <c r="F12" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A12)),"",MID(A12,FIND("title =",A12)+9,FIND("}",A12,FIND("title =",A12))-FIND("title =",A12)-9)),"")</f>
-        <v>Determinants of physical activity maintenance: a systematic review and meta-analyses</v>
-      </c>
-      <c r="G12" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A12, SEARCH("doi = {", A12) + 7, FIND("}", A12, SEARCH("doi = {", A12)) - SEARCH("doi = {", A12) - 7),"")</f>
-        <v>https://doi.org/10.1080/17437199.2012.701060</v>
-      </c>
-      <c r="H12" s="15">
-        <f ca="1">IF(A12&lt;&gt;"",IF(H12&lt;&gt;"",H12,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="36" customHeight="1">
-      <c r="A13" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A13, SEARCH("{", A13) + 1, SEARCH(",", A13) - SEARCH("{", A13) - 1), "")</f>
-        <v>@Roordink2021</v>
-      </c>
-      <c r="C13" s="10" t="str">
-        <f>"[" &amp; B13 &amp; "]"</f>
-        <v>[@Roordink2021]</v>
-      </c>
-      <c r="D13" s="11" t="str">
-        <f>IFERROR(MID(A13,SEARCH("year = {",A13)+8,4), "")</f>
-        <v>2021</v>
-      </c>
-      <c r="E13" s="11" t="str">
-        <f>IFERROR(MID(A13, SEARCH("author = {", A13) + 10, SEARCH("}", A13, SEARCH("author = {", A13)) - SEARCH("author = {", A13) - 10), "")</f>
-        <v>Roordink,  Eline M. and Steenhuis,  Ingrid H. M. and Kroeze,  Willemieke and Schoonmade,  Linda J. and Sniehotta,  Falko F. and van Stralen,  Maartje M.</v>
-      </c>
-      <c r="F13" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A13)),"",MID(A13,FIND("title =",A13)+9,FIND("},",A13,FIND("title =",A13))-FIND("title =",A13)-9)),"")</f>
-        <v>Predictors of lapse and relapse in physical activity and dietary behaviour: a systematic search and review on prospective studies</v>
-      </c>
-      <c r="G13" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A13, SEARCH("doi = {", A13) + 7, FIND("}", A13, SEARCH("doi = {", A13)) - SEARCH("doi = {", A13) - 7),"")</f>
-        <v>https://doi.org/10.1080/08870446.2021.1981900</v>
-      </c>
-      <c r="H13" s="15">
-        <f ca="1">IF(A13&lt;&gt;"",IF(H13&lt;&gt;"",H13,NOW()),"")</f>
-        <v>45588.888968865744</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="36" customHeight="1">
-      <c r="A14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A14, SEARCH("{", A14) + 1, SEARCH(",", A14) - SEARCH("{", A14) - 1), "")</f>
-        <v>@Gilchrist2018Pride</v>
-      </c>
-      <c r="C14" s="10" t="str">
-        <f>"[" &amp; B14 &amp; "]"</f>
-        <v>[@Gilchrist2018Pride]</v>
-      </c>
-      <c r="D14" s="11" t="str">
-        <f>IFERROR(MID(A14,SEARCH("year = {",A14)+8,4), "")</f>
-        <v>2018</v>
-      </c>
-      <c r="E14" s="11" t="str">
-        <f>IFERROR(MID(A14, SEARCH("author = {", A14) + 10, SEARCH("}", A14, SEARCH("author = {", A14)) - SEARCH("author = {", A14) - 10), "")</f>
-        <v>Gilchrist,  Jenna D. and Sabiston,  Catherine M. and Conroy,  David E. and Atkinson,  Michael</v>
-      </c>
-      <c r="F14" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A14)),"",MID(A14,FIND("title =",A14)+9,FIND("},",A14,FIND("title =",A14))-FIND("title =",A14)-9)),"")</f>
-        <v>Authentic pride regulates runners’ training progress</v>
-      </c>
-      <c r="G14" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A14, SEARCH("doi = {", A14) + 7, FIND("}", A14, SEARCH("doi = {", A14)) - SEARCH("doi = {", A14) - 7),"")</f>
-        <v>https://doi.org/10.1016/j.psychsport.2018.05.007</v>
-      </c>
-      <c r="H14" s="15">
-        <f ca="1">IF(A14&lt;&gt;"",IF(H14&lt;&gt;"",H14,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="36" customHeight="1">
-      <c r="A15" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A15, SEARCH("{", A15) + 1, SEARCH(",", A15) - SEARCH("{", A15) - 1), "")</f>
-        <v>@Gilchrist2018Grit</v>
-      </c>
-      <c r="C15" s="10" t="str">
-        <f>"[" &amp; B15 &amp; "]"</f>
-        <v>[@Gilchrist2018Grit]</v>
-      </c>
-      <c r="D15" s="11" t="str">
-        <f>IFERROR(MID(A15,SEARCH("year = {",A15)+8,4), "")</f>
-        <v>2018</v>
-      </c>
-      <c r="E15" s="11" t="str">
-        <f>IFERROR(MID(A15, SEARCH("author = {", A15) + 10, SEARCH("}", A15, SEARCH("author = {", A15)) - SEARCH("author = {", A15) - 10), "")</f>
-        <v>Gilchrist, Jenna D. and Fong, Angela J. and Herbison, Jordan D. and Sabiston, Catherine M.</v>
-      </c>
-      <c r="F15" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A15)),"",MID(A15,FIND("title =",A15)+9,FIND("},",A15,FIND("title =",A15))-FIND("title =",A15)-9)),"")</f>
-        <v>Feelings of pride are associated with grit in student-athletes and recreational runners</v>
-      </c>
-      <c r="G15" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A15, SEARCH("doi = {", A15) + 7, FIND("}", A15, SEARCH("doi = {", A15)) - SEARCH("doi = {", A15) - 7),"")</f>
-        <v>https://doi.org/10.1016/J.PSYCHSPORT.2017.12.009</v>
-      </c>
-      <c r="H15" s="15">
-        <f ca="1">IF(A15&lt;&gt;"",IF(H15&lt;&gt;"",H15,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="36" customHeight="1">
-      <c r="A16" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A16, SEARCH("{", A16) + 1, SEARCH(",", A16) - SEARCH("{", A16) - 1), "")</f>
-        <v>@Mack2015</v>
-      </c>
-      <c r="C16" s="10" t="str">
-        <f>"[" &amp; B16 &amp; "]"</f>
-        <v>[@Mack2015]</v>
-      </c>
-      <c r="D16" s="11" t="str">
-        <f>IFERROR(MID(A16,SEARCH("year = {",A16)+8,4), "")</f>
-        <v>2015</v>
-      </c>
-      <c r="E16" s="11" t="str">
-        <f>IFERROR(MID(A16, SEARCH("author = {", A16) + 10, SEARCH("}", A16, SEARCH("author = {", A16)) - SEARCH("author = {", A16) - 10), "")</f>
-        <v>Mack,  Diane E. and Kouali,  Despina and Gilchrist,  Jenna D. and Sabiston,  Catherine M.</v>
-      </c>
-      <c r="F16" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A16)),"",MID(A16,FIND("title =",A16)+9,FIND("}",A16,FIND("title =",A16))-FIND("title =",A16)-9)),"")</f>
-        <v>Pride and physical activity: Behavioural regulations as a motivational mechanism?</v>
-      </c>
-      <c r="G16" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A16, SEARCH("doi = {", A16) + 7, FIND("}", A16, SEARCH("doi = {", A16)) - SEARCH("doi = {", A16) - 7),"")</f>
-        <v>https://doi.org/10.1080/08870446.2015.1022547</v>
-      </c>
-      <c r="H16" s="15">
-        <f ca="1">IF(A16&lt;&gt;"",IF(H16&lt;&gt;"",H16,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="36" customHeight="1">
-      <c r="A17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A17, SEARCH("{", A17) + 1, SEARCH(",", A17) - SEARCH("{", A17) - 1), "")</f>
-        <v>@Tracy2007</v>
-      </c>
-      <c r="C17" s="10" t="str">
-        <f>"[" &amp; B17 &amp; "]"</f>
-        <v>[@Tracy2007]</v>
-      </c>
-      <c r="D17" s="11" t="str">
-        <f>IFERROR(MID(A17,SEARCH("year = {",A17)+8,4), "")</f>
-        <v>2007</v>
-      </c>
-      <c r="E17" s="11" t="str">
-        <f>IFERROR(MID(A17, SEARCH("author = {", A17) + 10, SEARCH("}", A17, SEARCH("author = {", A17)) - SEARCH("author = {", A17) - 10), "")</f>
-        <v>Tracy,  Jessica L. and Robins,  Richard W.</v>
-      </c>
-      <c r="F17" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A17)),"",MID(A17,FIND("title =",A17)+9,FIND("},",A17,FIND("title =",A17))-FIND("title =",A17)-9)),"")</f>
-        <v>Authentic And Hubristic Pride Scales</v>
-      </c>
-      <c r="G17" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A17, SEARCH("doi = {", A17) + 7, FIND("}", A17, SEARCH("doi = {", A17)) - SEARCH("doi = {", A17) - 7),"")</f>
-        <v>https://doi.org/10.1037/t06465-000</v>
-      </c>
-      <c r="H17" s="15">
-        <f ca="1">IF(A17&lt;&gt;"",IF(H17&lt;&gt;"",H17,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="36" customHeight="1">
-      <c r="A18" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A18, SEARCH("{", A18) + 1, SEARCH(",", A18) - SEARCH("{", A18) - 1), "")</f>
-        <v>@Marcus1997</v>
-      </c>
-      <c r="C18" s="10" t="str">
-        <f>"[" &amp; B18 &amp; "]"</f>
-        <v>[@Marcus1997]</v>
-      </c>
-      <c r="D18" s="11" t="str">
-        <f>IFERROR(MID(A18,SEARCH("year = {",A18)+8,4), "")</f>
-        <v>1997</v>
-      </c>
-      <c r="E18" s="11" t="str">
-        <f>IFERROR(MID(A18, SEARCH("author = {", A18) + 10, SEARCH("}", A18, SEARCH("author = {", A18)) - SEARCH("author = {", A18) - 10), "")</f>
-        <v>Marcus,  Bess H. and Bock,  Beth C. and Pinto,  Bernardine M.</v>
-      </c>
-      <c r="F18" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A18)),"",MID(A18,FIND("title =",A18)+9,FIND("}",A18,FIND("title =",A18))-FIND("title =",A18)-9)),"")</f>
-        <v>Initiation and Maintenance of Exercise Behavior</v>
-      </c>
-      <c r="G18" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A18, SEARCH("doi = {", A18) + 7, FIND("}", A18, SEARCH("doi = {", A18)) - SEARCH("doi = {", A18) - 7),"")</f>
-        <v>https://doi.org/10.1007/978-1-4899-1760-7_18</v>
-      </c>
-      <c r="H18" s="15">
-        <f ca="1">IF(A18&lt;&gt;"",IF(H18&lt;&gt;"",H18,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="36" customHeight="1">
-      <c r="A19" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A19, SEARCH("{", A19) + 1, SEARCH(",", A19) - SEARCH("{", A19) - 1), "")</f>
-        <v>@Marcus1993</v>
-      </c>
-      <c r="C19" s="10" t="str">
-        <f>"[" &amp; B19 &amp; "]"</f>
-        <v>[@Marcus1993]</v>
-      </c>
-      <c r="D19" s="11" t="str">
-        <f>IFERROR(MID(A19,SEARCH("year = {",A19)+8,4), "")</f>
-        <v>1993</v>
-      </c>
-      <c r="E19" s="11" t="str">
-        <f>IFERROR(MID(A19, SEARCH("author = {", A19) + 10, SEARCH("}", A19, SEARCH("author = {", A19)) - SEARCH("author = {", A19) - 10), "")</f>
-        <v>Marcus,  Bess H. and Stanton,  Annette L.</v>
-      </c>
-      <c r="F19" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A19)),"",MID(A19,FIND("title =",A19)+9,FIND("}",A19,FIND("title =",A19))-FIND("title =",A19)-9)),"")</f>
-        <v>Evaluation of Relapse Prevention and Reinforcement Interventions to Promote Exercise Adherence in Sedentary Females</v>
-      </c>
-      <c r="G19" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A19, SEARCH("doi = {", A19) + 7, FIND("}", A19, SEARCH("doi = {", A19)) - SEARCH("doi = {", A19) - 7),"")</f>
-        <v>https://doi.org/10.1080/02701367.1993.10607598</v>
-      </c>
-      <c r="H19" s="15">
-        <f ca="1">IF(A19&lt;&gt;"",IF(H19&lt;&gt;"",H19,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="36" customHeight="1">
-      <c r="A20" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A20, SEARCH("{", A20) + 1, SEARCH(",", A20) - SEARCH("{", A20) - 1), "")</f>
-        <v>@Martin1984</v>
-      </c>
-      <c r="C20" s="10" t="str">
-        <f>"[" &amp; B20 &amp; "]"</f>
-        <v>[@Martin1984]</v>
-      </c>
-      <c r="D20" s="11" t="str">
-        <f>IFERROR(MID(A20,SEARCH("year = {",A20)+8,4), "")</f>
-        <v>1984</v>
-      </c>
-      <c r="E20" s="11" t="str">
-        <f>IFERROR(MID(A20, SEARCH("author = {", A20) + 10, SEARCH("}", A20, SEARCH("author = {", A20)) - SEARCH("author = {", A20) - 10), "")</f>
-        <v>Martin,  John e. and Dubbert,  Patricia M. and Katell,  Alan D. and Thompson,  J. Kevin and Raczynski,  James R. and Lake,  Mary and Smith,  Patrick O. and Webster,  Jeffrey S. and Sikora,  Thomas and Cohen,  Randye E.</v>
-      </c>
-      <c r="F20" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A20)),"",MID(A20,FIND("title =",A20)+9,FIND("}",A20,FIND("title =",A20))-FIND("title =",A20)-9)),"")</f>
-        <v>Behavioral control of exercise in sedentary adults: Studies 1 through 6.</v>
-      </c>
-      <c r="G20" s="14" t="str">
-        <f>IFERROR("https://doi.org/" &amp; MID(A20, SEARCH("doi = {", A20) + 7, FIND("}", A20, SEARCH("doi = {", A20)) - SEARCH("doi = {", A20) - 7),"")</f>
-        <v>https://doi.org/10.1037/0022-006x.52.5.795</v>
-      </c>
-      <c r="H20" s="15">
-        <f ca="1">IF(A20&lt;&gt;"",IF(H20&lt;&gt;"",H20,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="36" customHeight="1">
-      <c r="A21" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="13" t="str">
-        <f>IFERROR("@" &amp; MID(A21, SEARCH("{", A21) + 1, SEARCH(",", A21) - SEARCH("{", A21) - 1), "")</f>
-        <v>@Stetson2005</v>
-      </c>
-      <c r="C21" s="10" t="str">
-        <f>"[" &amp; B21 &amp; "]"</f>
-        <v>[@Stetson2005]</v>
-      </c>
-      <c r="D21" s="11" t="str">
-        <f>IFERROR(MID(A21,SEARCH("year = {",A21)+8,4), "")</f>
-        <v>2005</v>
-      </c>
-      <c r="E21" s="11" t="str">
-        <f>IFERROR(MID(A21, SEARCH("author = {", A21) + 10, SEARCH("}", A21, SEARCH("author = {", A21)) - SEARCH("author = {", A21) - 10), "")</f>
-        <v>Stetson,  Barbara A. and Beacham,  Abbie O. and Frommelt,  Stephen J. and Boutelle,  Kerri N. and Cole,  Jonathan D. and Ziegler,  Craig H. and Looney,  Stephen W.</v>
-      </c>
-      <c r="F21" s="12" t="str">
-        <f>IFERROR(IF(ISERROR(FIND("title =",A21)),"",MID(A21,FIND("title =",A21)+9,FIND("}",A21,FIND("title =",A21))-FIND("title =",A21)-9)),"")</f>
-        <v>Exercise slips in high-risk situations and activity patterns in long-term exercisers: An application of the relapse prevention model</v>
       </c>
       <c r="G21" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A21, SEARCH("doi = {", A21) + 7, FIND("}", A21, SEARCH("doi = {", A21)) - SEARCH("doi = {", A21) - 7),"")</f>
-        <v>https://doi.org/10.1207/s15324796abm3001_4</v>
+        <v>https://doi.org/10.1007/978-3-531-19063-1_5</v>
       </c>
       <c r="H21" s="15">
         <f ca="1">IF(A21&lt;&gt;"",IF(H21&lt;&gt;"",H21,NOW()),"")</f>
-        <v>45580.951379513892</v>
+        <v>45581.517357060184</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="K21" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="36" customHeight="1">
       <c r="A22" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B22" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A22, SEARCH("{", A22) + 1, SEARCH(",", A22) - SEARCH("{", A22) - 1), "")</f>
-        <v>@lme4</v>
+        <v>@Roordink2021</v>
       </c>
       <c r="C22" s="10" t="str">
         <f>"[" &amp; B22 &amp; "]"</f>
-        <v>[@lme4]</v>
+        <v>[@Roordink2021]</v>
       </c>
       <c r="D22" s="11" t="str">
         <f>IFERROR(MID(A22,SEARCH("year = {",A22)+8,4), "")</f>
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="E22" s="11" t="str">
         <f>IFERROR(MID(A22, SEARCH("author = {", A22) + 10, SEARCH("}", A22, SEARCH("author = {", A22)) - SEARCH("author = {", A22) - 10), "")</f>
-        <v>Douglas Bates and Martin Mächler and Ben Bolker and Steve Walker</v>
+        <v>Roordink,  Eline M. and Steenhuis,  Ingrid H. M. and Kroeze,  Willemieke and Schoonmade,  Linda J. and Sniehotta,  Falko F. and van Stralen,  Maartje M.</v>
       </c>
       <c r="F22" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A22)),"",MID(A22,FIND("title =",A22)+9,FIND("},",A22,FIND("title =",A22))-FIND("title =",A22)-9)),"")</f>
-        <v>Fitting Linear Mixed-Effects Models Using {{lme4}}</v>
+        <v>Predictors of lapse and relapse in physical activity and dietary behaviour: a systematic search and review on prospective studies</v>
       </c>
       <c r="G22" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A22, SEARCH("doi = {", A22) + 7, FIND("}", A22, SEARCH("doi = {", A22)) - SEARCH("doi = {", A22) - 7),"")</f>
-        <v>https://doi.org/10.18637/jss.v067.i01</v>
+        <v>https://doi.org/10.1080/08870446.2021.1981900</v>
       </c>
       <c r="H22" s="15">
         <f ca="1">IF(A22&lt;&gt;"",IF(H22&lt;&gt;"",H22,NOW()),"")</f>
-        <v>45580.951379513892</v>
-      </c>
-      <c r="I22" s="1"/>
+        <v>45588.888968865744</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="36" customHeight="1">
       <c r="A23" s="17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A23, SEARCH("{", A23) + 1, SEARCH(",", A23) - SEARCH("{", A23) - 1), "")</f>
-        <v>@Marlatt1984</v>
+        <v>@Piggin2020</v>
       </c>
       <c r="C23" s="10" t="str">
         <f>"[" &amp; B23 &amp; "]"</f>
-        <v>[@Marlatt1984]</v>
+        <v>[@Piggin2020]</v>
       </c>
       <c r="D23" s="11" t="str">
         <f>IFERROR(MID(A23,SEARCH("year = {",A23)+8,4), "")</f>
-        <v>1984</v>
+        <v>2020</v>
       </c>
       <c r="E23" s="11" t="str">
         <f>IFERROR(MID(A23, SEARCH("author = {", A23) + 10, SEARCH("}", A23, SEARCH("author = {", A23)) - SEARCH("author = {", A23) - 10), "")</f>
-        <v>Marlatt,  G. Alan and George,  William H.</v>
+        <v>Piggin,  Joe</v>
       </c>
       <c r="F23" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A23)),"",MID(A23,FIND("title =",A23)+9,FIND("},",A23,FIND("title =",A23))-FIND("title =",A23)-9)),"")</f>
-        <v>Relapse Prevention: Introduction and Overview of the Model</v>
+        <v>What Is Physical Activity? A Holistic Definition for Teachers,  Researchers and Policy Makers</v>
       </c>
       <c r="G23" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A23, SEARCH("doi = {", A23) + 7, FIND("}", A23, SEARCH("doi = {", A23)) - SEARCH("doi = {", A23) - 7),"")</f>
-        <v>https://doi.org/10.1111/j.1360-0443.1984.tb03867.x</v>
+        <v>https://doi.org/10.3389/fspor.2020.00072</v>
       </c>
       <c r="H23" s="15">
         <f ca="1">IF(A23&lt;&gt;"",IF(H23&lt;&gt;"",H23,NOW()),"")</f>
-        <v>45580.951379513892</v>
+        <v>45588.905975462963</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="28" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="K23" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="36" customHeight="1">
       <c r="A24" s="17" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B24" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A24, SEARCH("{", A24) + 1, SEARCH(",", A24) - SEARCH("{", A24) - 1), "")</f>
-        <v>@Piggin2020</v>
+        <v>@caspersen1985physical</v>
       </c>
       <c r="C24" s="10" t="str">
         <f>"[" &amp; B24 &amp; "]"</f>
-        <v>[@Piggin2020]</v>
+        <v>[@caspersen1985physical]</v>
       </c>
       <c r="D24" s="11" t="str">
         <f>IFERROR(MID(A24,SEARCH("year = {",A24)+8,4), "")</f>
-        <v>2020</v>
+        <v>1985</v>
       </c>
       <c r="E24" s="11" t="str">
         <f>IFERROR(MID(A24, SEARCH("author = {", A24) + 10, SEARCH("}", A24, SEARCH("author = {", A24)) - SEARCH("author = {", A24) - 10), "")</f>
-        <v>Piggin,  Joe</v>
+        <v>Caspersen, Carl J. and Powell, Kenneth E. and Christenson, Gregory M.</v>
       </c>
       <c r="F24" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A24)),"",MID(A24,FIND("title =",A24)+9,FIND("},",A24,FIND("title =",A24))-FIND("title =",A24)-9)),"")</f>
-        <v>What Is Physical Activity? A Holistic Definition for Teachers,  Researchers and Policy Makers</v>
+        <v>Physical activity, exercise, and physical fitness: definitions and distinctions for health-related research</v>
       </c>
       <c r="G24" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A24, SEARCH("doi = {", A24) + 7, FIND("}", A24, SEARCH("doi = {", A24)) - SEARCH("doi = {", A24) - 7),"")</f>
-        <v>https://doi.org/10.3389/fspor.2020.00072</v>
+        <v/>
       </c>
       <c r="H24" s="15">
         <f ca="1">IF(A24&lt;&gt;"",IF(H24&lt;&gt;"",H24,NOW()),"")</f>
-        <v>45588.905975462963</v>
+        <v>45588.909048263886</v>
       </c>
       <c r="I24" s="1"/>
-      <c r="J24" s="28" t="s">
-        <v>54</v>
-      </c>
       <c r="K24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="36" customHeight="1">
       <c r="A25" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B25" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A25, SEARCH("{", A25) + 1, SEARCH(",", A25) - SEARCH("{", A25) - 1), "")</f>
-        <v>@caspersen1985physical</v>
+        <v>@Krug2013</v>
       </c>
       <c r="C25" s="10" t="str">
         <f>"[" &amp; B25 &amp; "]"</f>
-        <v>[@caspersen1985physical]</v>
+        <v>[@Krug2013]</v>
       </c>
       <c r="D25" s="11" t="str">
         <f>IFERROR(MID(A25,SEARCH("year = {",A25)+8,4), "")</f>
-        <v>1985</v>
+        <v>2013</v>
       </c>
       <c r="E25" s="11" t="str">
         <f>IFERROR(MID(A25, SEARCH("author = {", A25) + 10, SEARCH("}", A25, SEARCH("author = {", A25)) - SEARCH("author = {", A25) - 10), "")</f>
-        <v>Caspersen, Carl J. and Powell, Kenneth E. and Christenson, Gregory M.</v>
+        <v>Krug, Susanne and Jordan, Susanne and Mensink, Gert and Müters, Stephan and Finger, Jonas and Lampert, Thomas</v>
       </c>
       <c r="F25" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A25)),"",MID(A25,FIND("title =",A25)+9,FIND("},",A25,FIND("title =",A25))-FIND("title =",A25)-9)),"")</f>
-        <v>Physical activity, exercise, and physical fitness: definitions and distinctions for health-related research</v>
+        <v>Körperliche Aktivität</v>
       </c>
       <c r="G25" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A25, SEARCH("doi = {", A25) + 7, FIND("}", A25, SEARCH("doi = {", A25)) - SEARCH("doi = {", A25) - 7),"")</f>
-        <v/>
+        <v>https://doi.org/10.1007/s00103-012-1661-6</v>
       </c>
       <c r="H25" s="15">
         <f ca="1">IF(A25&lt;&gt;"",IF(H25&lt;&gt;"",H25,NOW()),"")</f>
-        <v>45588.909048263886</v>
+        <v>45588.940661342589</v>
       </c>
       <c r="I25" s="1"/>
       <c r="K25" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="120" customHeight="1">
       <c r="A26" s="17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B26" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A26, SEARCH("{", A26) + 1, SEARCH(",", A26) - SEARCH("{", A26) - 1), "")</f>
-        <v>@Krug2013</v>
+        <v>@Ainsworth2020</v>
       </c>
       <c r="C26" s="10" t="str">
         <f>"[" &amp; B26 &amp; "]"</f>
-        <v>[@Krug2013]</v>
+        <v>[@Ainsworth2020]</v>
       </c>
       <c r="D26" s="11" t="str">
         <f>IFERROR(MID(A26,SEARCH("year = {",A26)+8,4), "")</f>
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="E26" s="11" t="str">
         <f>IFERROR(MID(A26, SEARCH("author = {", A26) + 10, SEARCH("}", A26, SEARCH("author = {", A26)) - SEARCH("author = {", A26) - 10), "")</f>
-        <v>Krug, Susanne and Jordan, Susanne and Mensink, Gert and Müters, Stephan and Finger, Jonas and Lampert, Thomas</v>
+        <v>Ainsworth, Barbara E. and Der Ananian, Cheryl</v>
       </c>
       <c r="F26" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A26)),"",MID(A26,FIND("title =",A26)+9,FIND("},",A26,FIND("title =",A26))-FIND("title =",A26)-9)),"")</f>
-        <v>Körperliche Aktivität</v>
+        <v>Physical Activity Promotion</v>
       </c>
       <c r="G26" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A26, SEARCH("doi = {", A26) + 7, FIND("}", A26, SEARCH("doi = {", A26)) - SEARCH("doi = {", A26) - 7),"")</f>
-        <v>https://doi.org/10.1007/s00103-012-1661-6</v>
+        <v>https://doi.org/doi.org/10.1002/9781119568124.ch37</v>
       </c>
       <c r="H26" s="15">
         <f ca="1">IF(A26&lt;&gt;"",IF(H26&lt;&gt;"",H26,NOW()),"")</f>
-        <v>45588.940661342589</v>
+        <v>45589.89381238426</v>
       </c>
       <c r="I26" s="1"/>
       <c r="K26" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="36" customHeight="1">
       <c r="A27" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B27" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A27, SEARCH("{", A27) + 1, SEARCH(",", A27) - SEARCH("{", A27) - 1), "")</f>
-        <v>@Ainsworth2020</v>
+        <v>@Mcauley1994</v>
       </c>
       <c r="C27" s="10" t="str">
         <f>"[" &amp; B27 &amp; "]"</f>
-        <v>[@Ainsworth2020]</v>
+        <v>[@Mcauley1994]</v>
       </c>
       <c r="D27" s="11" t="str">
         <f>IFERROR(MID(A27,SEARCH("year = {",A27)+8,4), "")</f>
-        <v>2020</v>
+        <v>1994</v>
       </c>
       <c r="E27" s="11" t="str">
         <f>IFERROR(MID(A27, SEARCH("author = {", A27) + 10, SEARCH("}", A27, SEARCH("author = {", A27)) - SEARCH("author = {", A27) - 10), "")</f>
-        <v>Ainsworth, Barbara E. and Der Ananian, Cheryl</v>
+        <v>Mcauley,  E. and Courneya,  K.S. and Rudolph,  D.L. and Lox,  C.L.</v>
       </c>
       <c r="F27" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A27)),"",MID(A27,FIND("title =",A27)+9,FIND("},",A27,FIND("title =",A27))-FIND("title =",A27)-9)),"")</f>
-        <v>Physical Activity Promotion</v>
+        <v>Enhancing Exercise Adherence in Middle-Aged Males and Females</v>
       </c>
       <c r="G27" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A27, SEARCH("doi = {", A27) + 7, FIND("}", A27, SEARCH("doi = {", A27)) - SEARCH("doi = {", A27) - 7),"")</f>
-        <v>https://doi.org/doi.org/10.1002/9781119568124.ch37</v>
+        <v>https://doi.org/10.1006/pmed.1994.1068</v>
       </c>
       <c r="H27" s="15">
         <f ca="1">IF(A27&lt;&gt;"",IF(H27&lt;&gt;"",H27,NOW()),"")</f>
-        <v>45589.89381238426</v>
+        <v>45589.933628009261</v>
       </c>
       <c r="I27" s="1"/>
+      <c r="J27" s="30" t="s">
+        <v>63</v>
+      </c>
       <c r="K27" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="36" customHeight="1">
       <c r="A28" s="17" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B28" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A28, SEARCH("{", A28) + 1, SEARCH(",", A28) - SEARCH("{", A28) - 1), "")</f>
-        <v>@Mcauley1994</v>
+        <v>@Buckworth2007</v>
       </c>
       <c r="C28" s="10" t="str">
         <f>"[" &amp; B28 &amp; "]"</f>
-        <v>[@Mcauley1994]</v>
+        <v>[@Buckworth2007]</v>
       </c>
       <c r="D28" s="11" t="str">
         <f>IFERROR(MID(A28,SEARCH("year = {",A28)+8,4), "")</f>
-        <v>1994</v>
+        <v>2007</v>
       </c>
       <c r="E28" s="11" t="str">
         <f>IFERROR(MID(A28, SEARCH("author = {", A28) + 10, SEARCH("}", A28, SEARCH("author = {", A28)) - SEARCH("author = {", A28) - 10), "")</f>
-        <v>Mcauley,  E. and Courneya,  K.S. and Rudolph,  D.L. and Lox,  C.L.</v>
+        <v>Buckworth, Janet and Dishman, Rodney K.</v>
       </c>
       <c r="F28" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A28)),"",MID(A28,FIND("title =",A28)+9,FIND("},",A28,FIND("title =",A28))-FIND("title =",A28)-9)),"")</f>
-        <v>Enhancing Exercise Adherence in Middle-Aged Males and Females</v>
+        <v>Exercise adherence</v>
       </c>
       <c r="G28" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A28, SEARCH("doi = {", A28) + 7, FIND("}", A28, SEARCH("doi = {", A28)) - SEARCH("doi = {", A28) - 7),"")</f>
-        <v>https://doi.org/10.1006/pmed.1994.1068</v>
+        <v>https://doi.org/10.1002/9781118270011</v>
       </c>
       <c r="H28" s="15">
         <f ca="1">IF(A28&lt;&gt;"",IF(H28&lt;&gt;"",H28,NOW()),"")</f>
-        <v>45589.933628009261</v>
+        <v>45589.939154398147</v>
       </c>
       <c r="I28" s="1"/>
-      <c r="J28" s="30" t="s">
-        <v>63</v>
-      </c>
+      <c r="J28" s="30"/>
       <c r="K28" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="36" customHeight="1">
       <c r="A29" s="17" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B29" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A29, SEARCH("{", A29) + 1, SEARCH(",", A29) - SEARCH("{", A29) - 1), "")</f>
-        <v>@Buckworth2007</v>
+        <v>@WHO2010</v>
       </c>
       <c r="C29" s="10" t="str">
         <f>"[" &amp; B29 &amp; "]"</f>
-        <v>[@Buckworth2007]</v>
+        <v>[@WHO2010]</v>
       </c>
       <c r="D29" s="11" t="str">
         <f>IFERROR(MID(A29,SEARCH("year = {",A29)+8,4), "")</f>
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="E29" s="11" t="str">
         <f>IFERROR(MID(A29, SEARCH("author = {", A29) + 10, SEARCH("}", A29, SEARCH("author = {", A29)) - SEARCH("author = {", A29) - 10), "")</f>
-        <v>Buckworth, Janet and Dishman, Rodney K.</v>
+        <v/>
       </c>
       <c r="F29" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A29)),"",MID(A29,FIND("title =",A29)+9,FIND("},",A29,FIND("title =",A29))-FIND("title =",A29)-9)),"")</f>
-        <v>Exercise adherence</v>
+        <v>Global Recommendations on Physical Activity for Health</v>
       </c>
       <c r="G29" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A29, SEARCH("doi = {", A29) + 7, FIND("}", A29, SEARCH("doi = {", A29)) - SEARCH("doi = {", A29) - 7),"")</f>
-        <v>https://doi.org/10.1002/9781118270011</v>
+        <v/>
       </c>
       <c r="H29" s="15">
         <f ca="1">IF(A29&lt;&gt;"",IF(H29&lt;&gt;"",H29,NOW()),"")</f>
-        <v>45589.939154398147</v>
+        <v>45589.946631712963</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="30"/>
-      <c r="K29" t="s">
-        <v>66</v>
-      </c>
     </row>
     <row r="30" spans="1:11" ht="36" customHeight="1">
       <c r="A30" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B30" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A30, SEARCH("{", A30) + 1, SEARCH(",", A30) - SEARCH("{", A30) - 1), "")</f>
-        <v>@WHO2010</v>
+        <v>@Ding2016</v>
       </c>
       <c r="C30" s="10" t="str">
         <f>"[" &amp; B30 &amp; "]"</f>
-        <v>[@WHO2010]</v>
+        <v>[@Ding2016]</v>
       </c>
       <c r="D30" s="11" t="str">
         <f>IFERROR(MID(A30,SEARCH("year = {",A30)+8,4), "")</f>
-        <v>2010</v>
+        <v>2016</v>
       </c>
       <c r="E30" s="11" t="str">
         <f>IFERROR(MID(A30, SEARCH("author = {", A30) + 10, SEARCH("}", A30, SEARCH("author = {", A30)) - SEARCH("author = {", A30) - 10), "")</f>
-        <v/>
+        <v>Ding,  Ding and Lawson,  Kenny D and Kolbe-Alexander,  Tracy L and Finkelstein,  Eric A and Katzmarzyk,  Peter T and van Mechelen,  Willem and Pratt,  Michael</v>
       </c>
       <c r="F30" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A30)),"",MID(A30,FIND("title =",A30)+9,FIND("},",A30,FIND("title =",A30))-FIND("title =",A30)-9)),"")</f>
-        <v>Global Recommendations on Physical Activity for Health</v>
+        <v>The economic burden of physical inactivity: a global analysis of major non-communicable diseases</v>
       </c>
       <c r="G30" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A30, SEARCH("doi = {", A30) + 7, FIND("}", A30, SEARCH("doi = {", A30)) - SEARCH("doi = {", A30) - 7),"")</f>
-        <v/>
+        <v>https://doi.org/10.1016/s0140-6736(16)30383-x</v>
       </c>
       <c r="H30" s="15">
         <f ca="1">IF(A30&lt;&gt;"",IF(H30&lt;&gt;"",H30,NOW()),"")</f>
-        <v>45589.946631712963</v>
+        <v>45591.874786342596</v>
       </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="30"/>
+      <c r="J30" s="30" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="36" customHeight="1">
       <c r="A31" s="17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B31" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A31, SEARCH("{", A31) + 1, SEARCH(",", A31) - SEARCH("{", A31) - 1), "")</f>
-        <v>@Ding2016</v>
+        <v>@Warburton2006</v>
       </c>
       <c r="C31" s="10" t="str">
         <f>"[" &amp; B31 &amp; "]"</f>
-        <v>[@Ding2016]</v>
+        <v>[@Warburton2006]</v>
       </c>
       <c r="D31" s="11" t="str">
         <f>IFERROR(MID(A31,SEARCH("year = {",A31)+8,4), "")</f>
-        <v>2016</v>
+        <v>2006</v>
       </c>
       <c r="E31" s="11" t="str">
         <f>IFERROR(MID(A31, SEARCH("author = {", A31) + 10, SEARCH("}", A31, SEARCH("author = {", A31)) - SEARCH("author = {", A31) - 10), "")</f>
-        <v>Ding,  Ding and Lawson,  Kenny D and Kolbe-Alexander,  Tracy L and Finkelstein,  Eric A and Katzmarzyk,  Peter T and van Mechelen,  Willem and Pratt,  Michael</v>
+        <v>Warburton,  D. E.R.</v>
       </c>
       <c r="F31" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A31)),"",MID(A31,FIND("title =",A31)+9,FIND("},",A31,FIND("title =",A31))-FIND("title =",A31)-9)),"")</f>
-        <v>The economic burden of physical inactivity: a global analysis of major non-communicable diseases</v>
+        <v>Health benefits of physical activity: the evidence</v>
       </c>
       <c r="G31" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A31, SEARCH("doi = {", A31) + 7, FIND("}", A31, SEARCH("doi = {", A31)) - SEARCH("doi = {", A31) - 7),"")</f>
-        <v>https://doi.org/10.1016/s0140-6736(16)30383-x</v>
+        <v>https://doi.org/10.1503/cmaj.051351</v>
       </c>
       <c r="H31" s="15">
         <f ca="1">IF(A31&lt;&gt;"",IF(H31&lt;&gt;"",H31,NOW()),"")</f>
-        <v>45591.874786342596</v>
+        <v>45591.886342361111</v>
       </c>
       <c r="I31" s="1"/>
       <c r="J31" s="30" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="36" customHeight="1">
       <c r="A32" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B32" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A32, SEARCH("{", A32) + 1, SEARCH(",", A32) - SEARCH("{", A32) - 1), "")</f>
-        <v>@Warburton2006</v>
+        <v>@Myers2004</v>
       </c>
       <c r="C32" s="10" t="str">
         <f>"[" &amp; B32 &amp; "]"</f>
-        <v>[@Warburton2006]</v>
+        <v>[@Myers2004]</v>
       </c>
       <c r="D32" s="11" t="str">
         <f>IFERROR(MID(A32,SEARCH("year = {",A32)+8,4), "")</f>
-        <v>2006</v>
+        <v>2004</v>
       </c>
       <c r="E32" s="11" t="str">
         <f>IFERROR(MID(A32, SEARCH("author = {", A32) + 10, SEARCH("}", A32, SEARCH("author = {", A32)) - SEARCH("author = {", A32) - 10), "")</f>
-        <v>Warburton,  D. E.R.</v>
+        <v>Myers,  Jonathan and Kaykha,  Amir and George,  Sheela and Abella,  Joshua and Zaheer,  Naima and Lear,  Scott and Yamazaki,  Takuya and Froelicher,  Victor</v>
       </c>
       <c r="F32" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A32)),"",MID(A32,FIND("title =",A32)+9,FIND("},",A32,FIND("title =",A32))-FIND("title =",A32)-9)),"")</f>
-        <v>Health benefits of physical activity: the evidence</v>
+        <v>Fitness versus physical activity patterns in predicting mortality in men</v>
       </c>
       <c r="G32" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A32, SEARCH("doi = {", A32) + 7, FIND("}", A32, SEARCH("doi = {", A32)) - SEARCH("doi = {", A32) - 7),"")</f>
-        <v>https://doi.org/10.1503/cmaj.051351</v>
+        <v>https://doi.org/10.1016/j.amjmed.2004.06.047</v>
       </c>
       <c r="H32" s="15">
         <f ca="1">IF(A32&lt;&gt;"",IF(H32&lt;&gt;"",H32,NOW()),"")</f>
-        <v>45591.886342361111</v>
+        <v>45591.900539236114</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="30" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="36" customHeight="1">
       <c r="A33" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B33" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A33, SEARCH("{", A33) + 1, SEARCH(",", A33) - SEARCH("{", A33) - 1), "")</f>
-        <v>@Myers2004</v>
+        <v>@Lee2012</v>
       </c>
       <c r="C33" s="10" t="str">
         <f>"[" &amp; B33 &amp; "]"</f>
-        <v>[@Myers2004]</v>
+        <v>[@Lee2012]</v>
       </c>
       <c r="D33" s="11" t="str">
         <f>IFERROR(MID(A33,SEARCH("year = {",A33)+8,4), "")</f>
-        <v>2004</v>
+        <v>2012</v>
       </c>
       <c r="E33" s="11" t="str">
         <f>IFERROR(MID(A33, SEARCH("author = {", A33) + 10, SEARCH("}", A33, SEARCH("author = {", A33)) - SEARCH("author = {", A33) - 10), "")</f>
-        <v>Myers,  Jonathan and Kaykha,  Amir and George,  Sheela and Abella,  Joshua and Zaheer,  Naima and Lear,  Scott and Yamazaki,  Takuya and Froelicher,  Victor</v>
+        <v>Lee,  I-Min and Shiroma,  Eric J and Lobelo,  Felipe and Puska,  Pekka and Blair,  Steven N and Katzmarzyk,  Peter T</v>
       </c>
       <c r="F33" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A33)),"",MID(A33,FIND("title =",A33)+9,FIND("},",A33,FIND("title =",A33))-FIND("title =",A33)-9)),"")</f>
-        <v>Fitness versus physical activity patterns in predicting mortality in men</v>
+        <v>Effect of physical inactivity on major non-communicable diseases worldwide: an analysis of burden of disease and life expectancy</v>
       </c>
       <c r="G33" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A33, SEARCH("doi = {", A33) + 7, FIND("}", A33, SEARCH("doi = {", A33)) - SEARCH("doi = {", A33) - 7),"")</f>
-        <v>https://doi.org/10.1016/j.amjmed.2004.06.047</v>
+        <v>https://doi.org/10.1016/s0140-6736(12)61031-9</v>
       </c>
       <c r="H33" s="15">
         <f ca="1">IF(A33&lt;&gt;"",IF(H33&lt;&gt;"",H33,NOW()),"")</f>
-        <v>45591.900539236114</v>
+        <v>45591.912688888886</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="30" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="36" customHeight="1">
       <c r="A34" s="17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B34" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A34, SEARCH("{", A34) + 1, SEARCH(",", A34) - SEARCH("{", A34) - 1), "")</f>
-        <v>@Lee2012</v>
+        <v>@Paluska2000</v>
       </c>
       <c r="C34" s="10" t="str">
         <f>"[" &amp; B34 &amp; "]"</f>
-        <v>[@Lee2012]</v>
+        <v>[@Paluska2000]</v>
       </c>
       <c r="D34" s="11" t="str">
         <f>IFERROR(MID(A34,SEARCH("year = {",A34)+8,4), "")</f>
-        <v>2012</v>
+        <v>2000</v>
       </c>
       <c r="E34" s="11" t="str">
         <f>IFERROR(MID(A34, SEARCH("author = {", A34) + 10, SEARCH("}", A34, SEARCH("author = {", A34)) - SEARCH("author = {", A34) - 10), "")</f>
-        <v>Lee,  I-Min and Shiroma,  Eric J and Lobelo,  Felipe and Puska,  Pekka and Blair,  Steven N and Katzmarzyk,  Peter T</v>
+        <v>Paluska,  Scott A. and Schwenk,  Thomas L.</v>
       </c>
       <c r="F34" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A34)),"",MID(A34,FIND("title =",A34)+9,FIND("},",A34,FIND("title =",A34))-FIND("title =",A34)-9)),"")</f>
-        <v>Effect of physical inactivity on major non-communicable diseases worldwide: an analysis of burden of disease and life expectancy</v>
+        <v>Physical Activity and Mental Health: Current Concepts</v>
       </c>
       <c r="G34" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A34, SEARCH("doi = {", A34) + 7, FIND("}", A34, SEARCH("doi = {", A34)) - SEARCH("doi = {", A34) - 7),"")</f>
-        <v>https://doi.org/10.1016/s0140-6736(12)61031-9</v>
+        <v>https://doi.org/10.2165/00007256-200029030-00003</v>
       </c>
       <c r="H34" s="15">
         <f ca="1">IF(A34&lt;&gt;"",IF(H34&lt;&gt;"",H34,NOW()),"")</f>
-        <v>45591.912688888886</v>
+        <v>45592.857124652779</v>
       </c>
       <c r="I34" s="1"/>
       <c r="J34" s="30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="36" customHeight="1">
       <c r="A35" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B35" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A35, SEARCH("{", A35) + 1, SEARCH(",", A35) - SEARCH("{", A35) - 1), "")</f>
-        <v>@Paluska2000</v>
+        <v>@Mikkelsen2017</v>
       </c>
       <c r="C35" s="10" t="str">
         <f>"[" &amp; B35 &amp; "]"</f>
-        <v>[@Paluska2000]</v>
+        <v>[@Mikkelsen2017]</v>
       </c>
       <c r="D35" s="11" t="str">
         <f>IFERROR(MID(A35,SEARCH("year = {",A35)+8,4), "")</f>
-        <v>2000</v>
+        <v>2017</v>
       </c>
       <c r="E35" s="11" t="str">
         <f>IFERROR(MID(A35, SEARCH("author = {", A35) + 10, SEARCH("}", A35, SEARCH("author = {", A35)) - SEARCH("author = {", A35) - 10), "")</f>
-        <v>Paluska,  Scott A. and Schwenk,  Thomas L.</v>
+        <v>Mikkelsen,  Kathleen and Stojanovska,  Lily and Polenakovic,  Momir and Bosevski,  Marijan and Apostolopoulos,  Vasso</v>
       </c>
       <c r="F35" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A35)),"",MID(A35,FIND("title =",A35)+9,FIND("},",A35,FIND("title =",A35))-FIND("title =",A35)-9)),"")</f>
-        <v>Physical Activity and Mental Health: Current Concepts</v>
+        <v>Exercise and mental health</v>
       </c>
       <c r="G35" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A35, SEARCH("doi = {", A35) + 7, FIND("}", A35, SEARCH("doi = {", A35)) - SEARCH("doi = {", A35) - 7),"")</f>
-        <v>https://doi.org/10.2165/00007256-200029030-00003</v>
+        <v>https://doi.org/10.1016/j.maturitas.2017.09.003</v>
       </c>
       <c r="H35" s="15">
         <f ca="1">IF(A35&lt;&gt;"",IF(H35&lt;&gt;"",H35,NOW()),"")</f>
-        <v>45592.857124652779</v>
+        <v>45592.857473842596</v>
       </c>
       <c r="I35" s="1"/>
-      <c r="J35" s="30" t="s">
-        <v>77</v>
+      <c r="K35" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="36" customHeight="1">
       <c r="A36" s="17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B36" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A36, SEARCH("{", A36) + 1, SEARCH(",", A36) - SEARCH("{", A36) - 1), "")</f>
-        <v>@Mikkelsen2017</v>
+        <v>@Carter2016</v>
       </c>
       <c r="C36" s="10" t="str">
         <f>"[" &amp; B36 &amp; "]"</f>
-        <v>[@Mikkelsen2017]</v>
+        <v>[@Carter2016]</v>
       </c>
       <c r="D36" s="11" t="str">
         <f>IFERROR(MID(A36,SEARCH("year = {",A36)+8,4), "")</f>
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E36" s="11" t="str">
         <f>IFERROR(MID(A36, SEARCH("author = {", A36) + 10, SEARCH("}", A36, SEARCH("author = {", A36)) - SEARCH("author = {", A36) - 10), "")</f>
-        <v>Mikkelsen,  Kathleen and Stojanovska,  Lily and Polenakovic,  Momir and Bosevski,  Marijan and Apostolopoulos,  Vasso</v>
+        <v>Carter,  Tim and Morres,  Ioannis D. and Meade,  Oonagh and Callaghan,  Patrick</v>
       </c>
       <c r="F36" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A36)),"",MID(A36,FIND("title =",A36)+9,FIND("},",A36,FIND("title =",A36))-FIND("title =",A36)-9)),"")</f>
-        <v>Exercise and mental health</v>
+        <v>The Effect of Exercise on Depressive Symptoms in Adolescents: A Systematic Review and Meta-Analysis</v>
       </c>
       <c r="G36" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A36, SEARCH("doi = {", A36) + 7, FIND("}", A36, SEARCH("doi = {", A36)) - SEARCH("doi = {", A36) - 7),"")</f>
-        <v>https://doi.org/10.1016/j.maturitas.2017.09.003</v>
+        <v>https://doi.org/10.1016/j.jaac.2016.04.016</v>
       </c>
       <c r="H36" s="15">
         <f ca="1">IF(A36&lt;&gt;"",IF(H36&lt;&gt;"",H36,NOW()),"")</f>
-        <v>45592.857473842596</v>
+        <v>45592.861726620373</v>
       </c>
       <c r="I36" s="1"/>
-      <c r="K36" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="37" spans="1:11" ht="36" customHeight="1">
       <c r="A37" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B37" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A37, SEARCH("{", A37) + 1, SEARCH(",", A37) - SEARCH("{", A37) - 1), "")</f>
-        <v>@Carter2016</v>
+        <v>@Gillison2009</v>
       </c>
       <c r="C37" s="10" t="str">
         <f>"[" &amp; B37 &amp; "]"</f>
-        <v>[@Carter2016]</v>
+        <v>[@Gillison2009]</v>
       </c>
       <c r="D37" s="11" t="str">
         <f>IFERROR(MID(A37,SEARCH("year = {",A37)+8,4), "")</f>
-        <v>2016</v>
+        <v>2009</v>
       </c>
       <c r="E37" s="11" t="str">
         <f>IFERROR(MID(A37, SEARCH("author = {", A37) + 10, SEARCH("}", A37, SEARCH("author = {", A37)) - SEARCH("author = {", A37) - 10), "")</f>
-        <v>Carter,  Tim and Morres,  Ioannis D. and Meade,  Oonagh and Callaghan,  Patrick</v>
+        <v>Gillison,  Fiona Bridget and Skevington,  Suzanne M. and Sato,  Ayana and Standage,  Martyn and Evangelidou,  Stella</v>
       </c>
       <c r="F37" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A37)),"",MID(A37,FIND("title =",A37)+9,FIND("},",A37,FIND("title =",A37))-FIND("title =",A37)-9)),"")</f>
-        <v>The Effect of Exercise on Depressive Symptoms in Adolescents: A Systematic Review and Meta-Analysis</v>
+        <v>The effects of exercise interventions on quality of life in clinical and healthy populations; a meta-analysis</v>
       </c>
       <c r="G37" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A37, SEARCH("doi = {", A37) + 7, FIND("}", A37, SEARCH("doi = {", A37)) - SEARCH("doi = {", A37) - 7),"")</f>
-        <v>https://doi.org/10.1016/j.jaac.2016.04.016</v>
+        <v>https://doi.org/10.1016/j.socscimed.2009.02.028</v>
       </c>
       <c r="H37" s="15">
         <f ca="1">IF(A37&lt;&gt;"",IF(H37&lt;&gt;"",H37,NOW()),"")</f>
-        <v>45592.861726620373</v>
+        <v>45593.794906365743</v>
       </c>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:11" ht="36" customHeight="1">
       <c r="A38" s="17" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B38" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A38, SEARCH("{", A38) + 1, SEARCH(",", A38) - SEARCH("{", A38) - 1), "")</f>
-        <v>@Gillison2009</v>
+        <v>@Foster2017</v>
       </c>
       <c r="C38" s="10" t="str">
         <f>"[" &amp; B38 &amp; "]"</f>
-        <v>[@Gillison2009]</v>
+        <v>[@Foster2017]</v>
       </c>
       <c r="D38" s="11" t="str">
         <f>IFERROR(MID(A38,SEARCH("year = {",A38)+8,4), "")</f>
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="E38" s="11" t="str">
         <f>IFERROR(MID(A38, SEARCH("author = {", A38) + 10, SEARCH("}", A38, SEARCH("author = {", A38)) - SEARCH("author = {", A38) - 10), "")</f>
-        <v>Gillison,  Fiona Bridget and Skevington,  Suzanne M. and Sato,  Ayana and Standage,  Martyn and Evangelidou,  Stella</v>
+        <v>Foster,  Carl and Rodriguez-Marroyo,  Jose A. and de Koning,  Jos J.</v>
       </c>
       <c r="F38" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A38)),"",MID(A38,FIND("title =",A38)+9,FIND("},",A38,FIND("title =",A38))-FIND("title =",A38)-9)),"")</f>
-        <v>The effects of exercise interventions on quality of life in clinical and healthy populations; a meta-analysis</v>
+        <v>Monitoring Training Loads: The Past,  the Present,  and the Future</v>
       </c>
       <c r="G38" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A38, SEARCH("doi = {", A38) + 7, FIND("}", A38, SEARCH("doi = {", A38)) - SEARCH("doi = {", A38) - 7),"")</f>
-        <v>https://doi.org/10.1016/j.socscimed.2009.02.028</v>
+        <v>https://doi.org/10.1123/ijspp.2016-0388</v>
       </c>
       <c r="H38" s="15">
         <f ca="1">IF(A38&lt;&gt;"",IF(H38&lt;&gt;"",H38,NOW()),"")</f>
-        <v>45593.794906365743</v>
-      </c>
-      <c r="I38" s="1"/>
+        <v>45594.792853472223</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="36" customHeight="1">
       <c r="A39" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B39" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A39, SEARCH("{", A39) + 1, SEARCH(",", A39) - SEARCH("{", A39) - 1), "")</f>
@@ -19433,15 +19498,15 @@
         <v>45594.799354050927</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="36" customHeight="1">
       <c r="A40" s="17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B40" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A40, SEARCH("{", A40) + 1, SEARCH(",", A40) - SEARCH("{", A40) - 1), "")</f>
@@ -19473,12 +19538,12 @@
       </c>
       <c r="I40" s="1"/>
       <c r="K40" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="36" customHeight="1">
       <c r="A41" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B41" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A41, SEARCH("{", A41) + 1, SEARCH(",", A41) - SEARCH("{", A41) - 1), "")</f>
@@ -19511,130 +19576,143 @@
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:11" ht="36" customHeight="1">
-      <c r="A42" s="17"/>
+      <c r="A42" s="17" t="s">
+        <v>88</v>
+      </c>
       <c r="B42" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A42, SEARCH("{", A42) + 1, SEARCH(",", A42) - SEARCH("{", A42) - 1), "")</f>
-        <v/>
+        <v>@Crawford2004</v>
       </c>
       <c r="C42" s="10" t="str">
         <f>"[" &amp; B42 &amp; "]"</f>
-        <v>[]</v>
+        <v>[@Crawford2004]</v>
       </c>
       <c r="D42" s="11" t="str">
         <f>IFERROR(MID(A42,SEARCH("year = {",A42)+8,4), "")</f>
-        <v/>
+        <v>2004</v>
       </c>
       <c r="E42" s="11" t="str">
         <f>IFERROR(MID(A42, SEARCH("author = {", A42) + 10, SEARCH("}", A42, SEARCH("author = {", A42)) - SEARCH("author = {", A42) - 10), "")</f>
-        <v/>
+        <v>Crawford,  John R. and Henry,  Julie D.</v>
       </c>
       <c r="F42" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A42)),"",MID(A42,FIND("title =",A42)+9,FIND("},",A42,FIND("title =",A42))-FIND("title =",A42)-9)),"")</f>
-        <v/>
+        <v>The Positive and Negative Affect Schedule (PANAS): Construct validity,  measurement properties and normative data in a large non‐clinical sample</v>
       </c>
       <c r="G42" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A42, SEARCH("doi = {", A42) + 7, FIND("}", A42, SEARCH("doi = {", A42)) - SEARCH("doi = {", A42) - 7),"")</f>
-        <v/>
-      </c>
-      <c r="H42" s="15" t="str">
+        <v>https://doi.org/10.1348/0144665031752934</v>
+      </c>
+      <c r="H42" s="15">
         <f ca="1">IF(A42&lt;&gt;"",IF(H42&lt;&gt;"",H42,NOW()),"")</f>
-        <v/>
+        <v>45595.373129629632</v>
       </c>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:11" ht="36" customHeight="1">
-      <c r="A43" s="17"/>
+      <c r="A43" s="17" t="s">
+        <v>89</v>
+      </c>
       <c r="B43" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A43, SEARCH("{", A43) + 1, SEARCH(",", A43) - SEARCH("{", A43) - 1), "")</f>
-        <v/>
+        <v>@Corr1996</v>
       </c>
       <c r="C43" s="10" t="str">
         <f>"[" &amp; B43 &amp; "]"</f>
-        <v>[]</v>
+        <v>[@Corr1996]</v>
       </c>
       <c r="D43" s="11" t="str">
         <f>IFERROR(MID(A43,SEARCH("year = {",A43)+8,4), "")</f>
-        <v/>
+        <v>1996</v>
       </c>
       <c r="E43" s="11" t="str">
         <f>IFERROR(MID(A43, SEARCH("author = {", A43) + 10, SEARCH("}", A43, SEARCH("author = {", A43)) - SEARCH("author = {", A43) - 10), "")</f>
-        <v/>
+        <v>Corr,  Philip J. and Gray,  Jeffrey A.</v>
       </c>
       <c r="F43" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A43)),"",MID(A43,FIND("title =",A43)+9,FIND("},",A43,FIND("title =",A43))-FIND("title =",A43)-9)),"")</f>
-        <v/>
+        <v>Structure and Validity of the Attributional Style Questionnaire: A Cross-Sample Comparison</v>
       </c>
       <c r="G43" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A43, SEARCH("doi = {", A43) + 7, FIND("}", A43, SEARCH("doi = {", A43)) - SEARCH("doi = {", A43) - 7),"")</f>
-        <v/>
-      </c>
-      <c r="H43" s="15" t="str">
+        <v>https://doi.org/10.1080/00223980.1996.9915038</v>
+      </c>
+      <c r="H43" s="15">
         <f ca="1">IF(A43&lt;&gt;"",IF(H43&lt;&gt;"",H43,NOW()),"")</f>
-        <v/>
-      </c>
-      <c r="I43" s="1"/>
+        <v>45595.399233101853</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K43" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="44" spans="1:11" ht="36" customHeight="1">
-      <c r="A44" s="17"/>
+      <c r="A44" s="17" t="s">
+        <v>91</v>
+      </c>
       <c r="B44" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A44, SEARCH("{", A44) + 1, SEARCH(",", A44) - SEARCH("{", A44) - 1), "")</f>
-        <v/>
+        <v>@winter1994manual</v>
       </c>
       <c r="C44" s="10" t="str">
         <f>"[" &amp; B44 &amp; "]"</f>
-        <v>[]</v>
+        <v>[@winter1994manual]</v>
       </c>
       <c r="D44" s="11" t="str">
         <f>IFERROR(MID(A44,SEARCH("year = {",A44)+8,4), "")</f>
-        <v/>
+        <v>1994</v>
       </c>
       <c r="E44" s="11" t="str">
         <f>IFERROR(MID(A44, SEARCH("author = {", A44) + 10, SEARCH("}", A44, SEARCH("author = {", A44)) - SEARCH("author = {", A44) - 10), "")</f>
-        <v/>
+        <v>Winter, David G</v>
       </c>
       <c r="F44" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A44)),"",MID(A44,FIND("title =",A44)+9,FIND("},",A44,FIND("title =",A44))-FIND("title =",A44)-9)),"")</f>
-        <v/>
+        <v>Manual for scoring motive imagery in running text:(Version 4.2)</v>
       </c>
       <c r="G44" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A44, SEARCH("doi = {", A44) + 7, FIND("}", A44, SEARCH("doi = {", A44)) - SEARCH("doi = {", A44) - 7),"")</f>
         <v/>
       </c>
-      <c r="H44" s="15" t="str">
+      <c r="H44" s="15">
         <f ca="1">IF(A44&lt;&gt;"",IF(H44&lt;&gt;"",H44,NOW()),"")</f>
-        <v/>
+        <v>45595.476213541668</v>
       </c>
       <c r="I44" s="1"/>
     </row>
     <row r="45" spans="1:11" ht="36" customHeight="1">
-      <c r="A45" s="17"/>
+      <c r="A45" s="17" t="s">
+        <v>92</v>
+      </c>
       <c r="B45" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A45, SEARCH("{", A45) + 1, SEARCH(",", A45) - SEARCH("{", A45) - 1), "")</f>
-        <v/>
+        <v>@Sokolowski2000</v>
       </c>
       <c r="C45" s="10" t="str">
         <f>"[" &amp; B45 &amp; "]"</f>
-        <v>[]</v>
+        <v>[@Sokolowski2000]</v>
       </c>
       <c r="D45" s="11" t="str">
         <f>IFERROR(MID(A45,SEARCH("year = {",A45)+8,4), "")</f>
-        <v/>
+        <v>2000</v>
       </c>
       <c r="E45" s="11" t="str">
         <f>IFERROR(MID(A45, SEARCH("author = {", A45) + 10, SEARCH("}", A45, SEARCH("author = {", A45)) - SEARCH("author = {", A45) - 10), "")</f>
-        <v/>
+        <v>Sokolowski,  Kurt and Schmalt,  Heinz-Dieter and Langens,  Thomas A. and Puca,  Rosa M.</v>
       </c>
       <c r="F45" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A45)),"",MID(A45,FIND("title =",A45)+9,FIND("},",A45,FIND("title =",A45))-FIND("title =",A45)-9)),"")</f>
-        <v/>
+        <v>Assessing Achievement,  Affiliation,  and Power Motives All at Once: The Multi-Motive Grid (MMG)</v>
       </c>
       <c r="G45" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A45, SEARCH("doi = {", A45) + 7, FIND("}", A45, SEARCH("doi = {", A45)) - SEARCH("doi = {", A45) - 7),"")</f>
-        <v/>
-      </c>
-      <c r="H45" s="15" t="str">
+        <v>https://doi.org/10.1207/s15327752jpa740109</v>
+      </c>
+      <c r="H45" s="15">
         <f ca="1">IF(A45&lt;&gt;"",IF(H45&lt;&gt;"",H45,NOW()),"")</f>
-        <v/>
+        <v>45595.47760150463</v>
       </c>
       <c r="I45" s="1"/>
     </row>
@@ -34280,7 +34358,7 @@
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R505">
-    <sortCondition ref="I2:I505"/>
+    <sortCondition ref="H2:H505"/>
   </sortState>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="1">
@@ -34303,21 +34381,22 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{8A25D788-B58A-4CF8-B464-1AAAEA0A1B9F}"/>
-    <hyperlink ref="J21" r:id="rId2" display="../../../../../../:b:/g/personal/enno_winkler_spb-ew_de/Ea29HBFCZ8FLnoGw4FFBbxYBjGh5Fq-CR36In5zFhIiU5g?e=UYtXYq" xr:uid="{A7FA5F64-9021-4490-9216-344727A2237F}"/>
-    <hyperlink ref="J23" r:id="rId3" display="../../../../../../:b:/g/personal/enno_winkler_spb-ew_de/ESOOt3KtIyFHibYstwiwCVABQ8BC3E7KOhWZU9Vi-Sjd8A?e=oNhrDv" xr:uid="{22B400D9-B494-40B1-9AD2-B3E9A7CAF00B}"/>
-    <hyperlink ref="J24" r:id="rId4" display="../../../../../../:b:/g/personal/enno_winkler_spb-ew_de/EUTaIvjDacJGjD07e_JcaTgBS1hpif-Gyhb4QQWlhX86vQ?e=m2EAh5" xr:uid="{81071813-5CF9-4DAE-9521-4C626ECFA18D}"/>
-    <hyperlink ref="J28" r:id="rId5" xr:uid="{0A9C2473-0409-4305-B3A7-49056702B7C0}"/>
-    <hyperlink ref="J31" r:id="rId6" xr:uid="{304BB387-01C5-4638-BBAB-99939BBCD0A3}"/>
-    <hyperlink ref="J32" r:id="rId7" xr:uid="{678649AF-5D7E-4ACA-8A7F-E9D34255A849}"/>
-    <hyperlink ref="J33" r:id="rId8" xr:uid="{1DFF1E7D-B6CF-46E4-8DDC-8041FD898A3E}"/>
-    <hyperlink ref="J34" r:id="rId9" xr:uid="{00B217BF-927C-4C6A-8DC3-DA0FD6972FFD}"/>
-    <hyperlink ref="J35" r:id="rId10" xr:uid="{6475CF80-FCA4-4093-BD94-7CDEAE4F05EF}"/>
+    <hyperlink ref="J21" r:id="rId1" xr:uid="{8A25D788-B58A-4CF8-B464-1AAAEA0A1B9F}"/>
+    <hyperlink ref="J16" r:id="rId2" display="https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/Exercise%20Slips%20in%20High-Risk%20Situations%20and%20Activity%20Patterns%20in%20Long-Term%20Exercisers.pdf?csf=1&amp;web=1&amp;e=geTkBC" xr:uid="{A7FA5F64-9021-4490-9216-344727A2237F}"/>
+    <hyperlink ref="J18" r:id="rId3" display="https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/British%20Journal%20of%20Addiction%20-%20December%201984%20-%20Marlatt%20-%20Relapse%20Prevention%20Introduction%20and%20Overview%20of%20the%20Model.pdf?csf=1&amp;web=1&amp;e=1bgEat" xr:uid="{22B400D9-B494-40B1-9AD2-B3E9A7CAF00B}"/>
+    <hyperlink ref="J23" r:id="rId4" xr:uid="{81071813-5CF9-4DAE-9521-4C626ECFA18D}"/>
+    <hyperlink ref="J27" r:id="rId5" xr:uid="{0A9C2473-0409-4305-B3A7-49056702B7C0}"/>
+    <hyperlink ref="J30" r:id="rId6" xr:uid="{304BB387-01C5-4638-BBAB-99939BBCD0A3}"/>
+    <hyperlink ref="J31" r:id="rId7" xr:uid="{678649AF-5D7E-4ACA-8A7F-E9D34255A849}"/>
+    <hyperlink ref="J32" r:id="rId8" xr:uid="{1DFF1E7D-B6CF-46E4-8DDC-8041FD898A3E}"/>
+    <hyperlink ref="J33" r:id="rId9" xr:uid="{00B217BF-927C-4C6A-8DC3-DA0FD6972FFD}"/>
+    <hyperlink ref="J34" r:id="rId10" xr:uid="{6475CF80-FCA4-4093-BD94-7CDEAE4F05EF}"/>
+    <hyperlink ref="J4" r:id="rId11" xr:uid="{A1DC44F4-3410-4EF5-B7AB-3A688E028A13}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId11"/>
-  <legacyDrawing r:id="rId12"/>
+  <drawing r:id="rId12"/>
+  <legacyDrawing r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -34333,15 +34412,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -34366,176 +34445,176 @@
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="72.75" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="32" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="23" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="180" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="210" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="255" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="255" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="285" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="285" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105" customHeight="1">
       <c r="A19" s="25" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120" customHeight="1">
       <c r="A20" s="25" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135" customHeight="1">
       <c r="A21" s="25" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
explanation for the relapse model + Hypothesis + research question
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit mit bindr/Markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CF8420D-5ADB-482F-A4C2-AA285B63E302}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62A4B9C8-DDF2-44FF-BAC0-468E6A2A5F18}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-5460" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="140">
   <si>
     <t>@article{example2024,   title = {A Reference Example},   journal = {Journal of Examples},   publisher = {Example Press},   author = {Doe, Jane},   year = {2024},   month = aug,   pages = {185–209} }</t>
   </si>
@@ -817,6 +817,15 @@
   year = {2000},
   month = feb,
   pages = {126–145}
+}</t>
+  </si>
+  <si>
+    <t>@book{bandura1977social,
+  title = {Social Learning Theory},
+  author = {Bandura, Albert},
+  year = {1977},
+  publisher = {Prentice-Hall},
+  address = {Englewood Cliffs, NJ},
 }</t>
   </si>
   <si>
@@ -18018,8 +18027,8 @@
   <dimension ref="A1:R505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="F9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -19717,34 +19726,36 @@
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:11" ht="36" customHeight="1">
-      <c r="A46" s="17"/>
+      <c r="A46" s="17" t="s">
+        <v>93</v>
+      </c>
       <c r="B46" s="13" t="str">
         <f>IFERROR("@" &amp; MID(A46, SEARCH("{", A46) + 1, SEARCH(",", A46) - SEARCH("{", A46) - 1), "")</f>
-        <v/>
+        <v>@bandura1977social</v>
       </c>
       <c r="C46" s="10" t="str">
         <f>"[" &amp; B46 &amp; "]"</f>
-        <v>[]</v>
+        <v>[@bandura1977social]</v>
       </c>
       <c r="D46" s="11" t="str">
         <f>IFERROR(MID(A46,SEARCH("year = {",A46)+8,4), "")</f>
-        <v/>
+        <v>1977</v>
       </c>
       <c r="E46" s="11" t="str">
         <f>IFERROR(MID(A46, SEARCH("author = {", A46) + 10, SEARCH("}", A46, SEARCH("author = {", A46)) - SEARCH("author = {", A46) - 10), "")</f>
-        <v/>
+        <v>Bandura, Albert</v>
       </c>
       <c r="F46" s="12" t="str">
         <f>IFERROR(IF(ISERROR(FIND("title =",A46)),"",MID(A46,FIND("title =",A46)+9,FIND("},",A46,FIND("title =",A46))-FIND("title =",A46)-9)),"")</f>
-        <v/>
+        <v>Social Learning Theory</v>
       </c>
       <c r="G46" s="14" t="str">
         <f>IFERROR("https://doi.org/" &amp; MID(A46, SEARCH("doi = {", A46) + 7, FIND("}", A46, SEARCH("doi = {", A46)) - SEARCH("doi = {", A46) - 7),"")</f>
         <v/>
       </c>
-      <c r="H46" s="15" t="str">
+      <c r="H46" s="15">
         <f ca="1">IF(A46&lt;&gt;"",IF(H46&lt;&gt;"",H46,NOW()),"")</f>
-        <v/>
+        <v>45620.901083680554</v>
       </c>
       <c r="I46" s="1"/>
     </row>
@@ -34412,15 +34423,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -34445,176 +34456,176 @@
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="72.75" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="23" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="180" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="210" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="255" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="255" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="285" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="285" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105" customHeight="1">
       <c r="A19" s="25" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120" customHeight="1">
       <c r="A20" s="25" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135" customHeight="1">
       <c r="A21" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- reporting hlm results
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit/Markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="174" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A3F6952-8D95-4B99-934B-0CCBBC5D36AF}"/>
+  <xr:revisionPtr revIDLastSave="178" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADB5FBE9-8829-403D-9EF4-231AFE279650}"/>
   <bookViews>
     <workbookView xWindow="-37230" yWindow="-4185" windowWidth="28800" windowHeight="15345" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="145">
   <si>
     <t>@article{example2024,   title = {A Reference Example},   journal = {Journal of Examples},   publisher = {Example Press},   author = {Doe, Jane},   year = {2024},   month = aug,   pages = {185–209} }</t>
   </si>
@@ -870,6 +870,30 @@
   month = nov,
   pages = {1966}
 }</t>
+  </si>
+  <si>
+    <t>@book{Cohen2013,
+  title = {Statistical Power Analysis for the Behavioral Sciences},
+  ISBN = {9781134742707},
+  url = {http://dx.doi.org/10.4324/9780203771587},
+  DOI = {10.4324/9780203771587},
+  publisher = {Routledge},
+  author = {Cohen,  Jacob},
+  year = {2013},
+  month = may 
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@article{nezlek2008introduction,
+  title = {An Introduction to Multilevel Modeling for Social and Personality Psychology},
+  author = {Nezlek, John B.},
+  year = {2008},
+  journal = {Social and Personality Psychology Compass},
+  volume = {2},
+  number = {2},
+  pages = {842--860},
+}
+</t>
   </si>
   <si>
     <t>Abbreviations</t>
@@ -18070,8 +18094,8 @@
   <dimension ref="A1:R505"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A52" sqref="A52:XFD52"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -19905,99 +19929,82 @@
       <c r="I49" s="1"/>
     </row>
     <row r="50" spans="1:9" ht="36" customHeight="1">
-      <c r="A50" s="17"/>
+      <c r="A50" s="17" t="s">
+        <v>97</v>
+      </c>
       <c r="B50" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@Cohen2013</v>
       </c>
       <c r="C50" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@Cohen2013]</v>
       </c>
       <c r="D50" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2013</v>
       </c>
       <c r="E50" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Cohen,  Jacob</v>
       </c>
       <c r="F50" s="12" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>Statistical Power Analysis for the Behavioral Sciences</v>
       </c>
       <c r="G50" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H50" s="15" t="str">
+        <v>https://doi.org/10.4324/9780203771587</v>
+      </c>
+      <c r="H50" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45651.849579166665</v>
       </c>
       <c r="I50" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="36" customHeight="1">
-      <c r="A51" s="17"/>
+      <c r="A51" s="17" t="s">
+        <v>98</v>
+      </c>
       <c r="B51" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@nezlek2008introduction</v>
       </c>
       <c r="C51" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@nezlek2008introduction]</v>
       </c>
       <c r="D51" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2008</v>
       </c>
       <c r="E51" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Nezlek, John B.</v>
       </c>
       <c r="F51" s="12" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>An Introduction to Multilevel Modeling for Social and Personality Psychology</v>
       </c>
       <c r="G51" s="14" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="H51" s="15" t="str">
+      <c r="H51" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45651.877939120372</v>
       </c>
       <c r="I51" s="1"/>
     </row>
     <row r="52" spans="1:9" ht="36" customHeight="1">
       <c r="A52" s="17"/>
-      <c r="B52" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C52" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>[]</v>
-      </c>
-      <c r="D52" s="11" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="E52" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="F52" s="12" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="G52" s="14" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H52" s="15" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v/>
-      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="15"/>
       <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:9" ht="36" customHeight="1">
@@ -34472,15 +34479,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -34505,176 +34512,176 @@
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="72.75" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="32" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="180" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="210" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="255" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="255" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="285" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="285" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105" customHeight="1">
       <c r="A19" s="25" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120" customHeight="1">
       <c r="A20" s="25" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135" customHeight="1">
       <c r="A21" s="25" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1 removed binder badge 2 added text in introduction 3 added tidy - method to the Regression analysis tables 4 renamed "Na_amount" to "missings_amount 5 deleted redundant files, fixed rendering issues
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28502"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ennosgermancourse-my.sharepoint.com/personal/enno_winkler_spb-ew_de/Documents/A Fernstudium Kursmaterial/Bachelorarbeit/Markdown/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E21A2D3-C501-40A4-8C22-CD34AF3A5C37}"/>
+  <xr:revisionPtr revIDLastSave="213" documentId="13_ncr:1_{5B3F93C2-1706-4273-9041-268344AC6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{370F5DBB-A560-4DB8-AF1E-38301EF6CC18}"/>
   <bookViews>
     <workbookView xWindow="-37230" yWindow="-4185" windowWidth="28800" windowHeight="15345" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="155">
   <si>
     <t>@article{example2024,   title = {A Reference Example},   journal = {Journal of Examples},   publisher = {Example Press},   author = {Doe, Jane},   year = {2024},   month = aug,   pages = {185–209} }</t>
   </si>
@@ -901,7 +901,7 @@
   author = {Ellis, Andrew and Mayer, Boris},
   year = {2020},
   url = {https://methodenlehre.github.io/intro-to-rstats/index.html},
-  note = {Accessed: [Insert access date]},
+  note = {Accessed: 2025-01-05}
 }</t>
   </si>
   <si>
@@ -913,7 +913,7 @@
     author = {José Pinheiro and Douglas Bates and {R Core Team}},
     year = {2023},
     note = {R package version 3.1-164},
-    url = {https://CRAN.R-project.org/package=nlme},
+    url = {https://CRAN.R-project.org/package=nlme}
   }</t>
   </si>
   <si>
@@ -925,7 +925,76 @@
     volume = {67},
     number = {1},
     pages = {1--48},
-    doi = {10.18637/jss.v067.i01},</t>
+    doi = {10.18637/jss.v067.i01}
+}</t>
+  </si>
+  <si>
+    <t>@article{Engel1977,
+  title = {The Need for a New Medical Model: A Challenge for Biomedicine},
+  volume = {196},
+  ISSN = {1095-9203},
+  url = {http://dx.doi.org/10.1126/science.847460},
+  DOI = {10.1126/science.847460},
+  number = {4286},
+  journal = {Science},
+  publisher = {American Association for the Advancement of Science (AAAS)},
+  author = {Engel,  George L.},
+  year = {1977},
+  month = apr,
+  pages = {129–136}
+}</t>
+  </si>
+  <si>
+    <t>@article{Ledochowski2016,
+  title = {K\"{o}rperliche Aktivit\"{a}t als therapeutische Intervention bei Depression},
+  volume = {88},
+  ISSN = {1433-0407},
+  url = {http://dx.doi.org/10.1007/s00115-016-0222-x},
+  DOI = {10.1007/s00115-016-0222-x},
+  number = {7},
+  journal = {Der Nervenarzt},
+  publisher = {Springer Science and Business Media LLC},
+  author = {Ledochowski,  L. and Stark,  R. and Ruedl,  G. and Kopp,  M.},
+  year = {2016},
+  month = sep,
+  pages = {765–778}
+}</t>
+  </si>
+  <si>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/Ledochowski_PA_depression.pdf?csf=1&amp;web=1&amp;e=wkbseE</t>
+  </si>
+  <si>
+    <t>@article{Cooney08,
+author = {Cooney, GM, Dwan, K, Greig, CA, Lawlor, DA, Rimer, J, Waugh, FR, McMurdo, M, and Mead, GE},
+title = {Exercise for depression},
+journal = {Cochrane Database of Systematic Reviews},
+number = {9},
+year = {2013},
+publisher = {John Wiley &amp; Sons, Ltd},
+ISSN = {1465-1858},
+DOI = {10.1002/14651858.CD004366.pub6},
+keywords = {Adult; Depression [*therapy]; Exercise [*psychology]; Humans; Middle Aged; Psychotherapy; Randomized Controlled Trials as Topic; Treatment Outcome; Young Adult},
+URL = {https://doi.org//10.1002/14651858.CD004366.pub6}
+}</t>
+  </si>
+  <si>
+    <t>@article{Morres2018,
+  title = {Aerobic exercise for adult patients with major depressive disorder in mental health services: A systematic review and meta-analysis},
+  volume = {36},
+  ISSN = {1091-4269},
+  url = {http://dx.doi.org/10.1002/da.22842},
+  DOI = {10.1002/da.22842},
+  number = {1},
+  journal = {Depression and Anxiety},
+  publisher = {Wiley},
+  author = {Morres,  Ioannis D. and Hatzigeorgiadis,  Antonis and Stathi,  Afroditi and Comoutos,  Nikos and Arpin-Cribbie,  Chantal and Krommidas,  Charalampos and Theodorakis,  Yannis},
+  year = {2018},
+  month = oct,
+  pages = {39–53}
+}</t>
+  </si>
+  <si>
+    <t>https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/Depression%20and%20Anxiety%20-%202018%20-%20Morres%20-%20Aerobic%20exercise%20for%20adult%20patients%20with%20major%20depressive%20disorder%20in%20mental.pdf?csf=1&amp;web=1&amp;e=Ov2lg8</t>
   </si>
   <si>
     <t>Abbreviations</t>
@@ -18126,8 +18195,8 @@
   <dimension ref="A1:R504"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -20134,132 +20203,146 @@
       <c r="I54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="36" customHeight="1">
-      <c r="A55" s="17"/>
+      <c r="A55" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="B55" s="13" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>@Engel1977</v>
       </c>
       <c r="C55" s="10" t="str">
         <f t="shared" si="8"/>
-        <v>[]</v>
+        <v>[@Engel1977]</v>
       </c>
       <c r="D55" s="11" t="str">
         <f t="shared" si="9"/>
-        <v/>
+        <v>1977</v>
       </c>
       <c r="E55" s="11" t="str">
         <f t="shared" si="10"/>
-        <v/>
+        <v>Engel,  George L.</v>
       </c>
       <c r="F55" s="12" t="str">
         <f t="shared" si="11"/>
-        <v/>
+        <v>The Need for a New Medical Model: A Challenge for Biomedicine</v>
       </c>
       <c r="G55" s="14" t="str">
         <f t="shared" si="12"/>
-        <v/>
-      </c>
-      <c r="H55" s="15" t="str">
+        <v>https://doi.org/10.1126/science.847460</v>
+      </c>
+      <c r="H55" s="15">
         <f t="shared" ca="1" si="13"/>
-        <v/>
+        <v>45666.50709525463</v>
       </c>
       <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:11" ht="36" customHeight="1">
-      <c r="A56" s="17"/>
+      <c r="A56" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="B56" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@Ledochowski2016</v>
       </c>
       <c r="C56" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@Ledochowski2016]</v>
       </c>
       <c r="D56" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2016</v>
       </c>
       <c r="E56" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Ledochowski,  L. and Stark,  R. and Ruedl,  G. and Kopp,  M.</v>
       </c>
       <c r="F56" s="12" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>K\"{o}rperliche Aktivit\"{a}t als therapeutische Intervention bei Depression</v>
       </c>
       <c r="G56" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H56" s="15" t="str">
+        <v>https://doi.org/10.1007/s00115-016-0222-x</v>
+      </c>
+      <c r="H56" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45666.699690624999</v>
       </c>
       <c r="I56" s="1"/>
+      <c r="J56" s="30" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="57" spans="1:11" ht="36" customHeight="1">
-      <c r="A57" s="17"/>
+      <c r="A57" s="17" t="s">
+        <v>106</v>
+      </c>
       <c r="B57" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@Cooney08</v>
       </c>
       <c r="C57" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@Cooney08]</v>
       </c>
       <c r="D57" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2013</v>
       </c>
       <c r="E57" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Cooney, GM, Dwan, K, Greig, CA, Lawlor, DA, Rimer, J, Waugh, FR, McMurdo, M, and Mead, GE</v>
       </c>
       <c r="F57" s="12" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>Exercise for depression</v>
       </c>
       <c r="G57" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H57" s="15" t="str">
+        <v>https://doi.org/10.1002/14651858.CD004366.pub6</v>
+      </c>
+      <c r="H57" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45666.705761226855</v>
       </c>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:11" ht="36" customHeight="1">
-      <c r="A58" s="17"/>
+      <c r="A58" s="17" t="s">
+        <v>107</v>
+      </c>
       <c r="B58" s="13" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>@Morres2018</v>
       </c>
       <c r="C58" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>[]</v>
+        <v>[@Morres2018]</v>
       </c>
       <c r="D58" s="11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>2018</v>
       </c>
       <c r="E58" s="11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Morres,  Ioannis D. and Hatzigeorgiadis,  Antonis and Stathi,  Afroditi and Comoutos,  Nikos and Arpin-Cribbie,  Chantal and Krommidas,  Charalampos and Theodorakis,  Yannis</v>
       </c>
       <c r="F58" s="12" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>Aerobic exercise for adult patients with major depressive disorder in mental health services: A systematic review and meta-analysis</v>
       </c>
       <c r="G58" s="14" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="H58" s="15" t="str">
+        <v>https://doi.org/10.1002/da.22842</v>
+      </c>
+      <c r="H58" s="15">
         <f t="shared" ca="1" si="5"/>
-        <v/>
+        <v>45666.710162152776</v>
       </c>
       <c r="I58" s="1"/>
+      <c r="J58" s="30" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="59" spans="1:11" ht="36" customHeight="1">
       <c r="A59" s="17"/>
@@ -34489,11 +34572,13 @@
     <hyperlink ref="J33" r:id="rId9" xr:uid="{00B217BF-927C-4C6A-8DC3-DA0FD6972FFD}"/>
     <hyperlink ref="J34" r:id="rId10" xr:uid="{6475CF80-FCA4-4093-BD94-7CDEAE4F05EF}"/>
     <hyperlink ref="J4" r:id="rId11" xr:uid="{A1DC44F4-3410-4EF5-B7AB-3A688E028A13}"/>
+    <hyperlink ref="J56" r:id="rId12" xr:uid="{8F180BD5-D022-4F73-BC6C-0CB060C9B675}"/>
+    <hyperlink ref="J58" r:id="rId13" display="https://ennosgermancourse-my.sharepoint.com/:b:/r/personal/enno_winkler_spb-ew_de/Documents/A%20Fernstudium%20Kursmaterial/Bachelorarbeit/Info/LIT/Depression%20and%20Anxiety%20-%202018%20-%20Morres%20-%20Aerobic%20exercise%20for%20adult%20patients%20with%20major%20depressive%20disorder%20in%20mental.pdf?csf=1&amp;web=1&amp;e=Ov2lg8" xr:uid="{FE167BEA-5841-4F90-AF79-5B38107D31D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId12"/>
-  <legacyDrawing r:id="rId13"/>
+  <drawing r:id="rId14"/>
+  <legacyDrawing r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -34509,15 +34594,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -34542,176 +34627,176 @@
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" customHeight="1">
       <c r="A1" s="31" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:3" ht="72.75" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="32" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="23" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="180" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" customHeight="1">
       <c r="A6" s="25" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="210" customHeight="1">
       <c r="A7" s="25" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="255" customHeight="1">
       <c r="A9" s="25" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="255" customHeight="1">
       <c r="A10" s="25" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="285" customHeight="1">
       <c r="A11" s="25" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="285" customHeight="1">
       <c r="A12" s="25" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1">
       <c r="A14" s="25" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165" customHeight="1">
       <c r="A15" s="25" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" customHeight="1">
       <c r="A16" s="25" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225" customHeight="1">
       <c r="A17" s="25" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105" customHeight="1">
       <c r="A19" s="25" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120" customHeight="1">
       <c r="A20" s="25" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135" customHeight="1">
       <c r="A21" s="25" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix: using the label tbl-glm caused an error
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -18211,8 +18211,8 @@
   <dimension ref="A1:R504"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+      <pane ySplit="1" topLeftCell="B43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tables and Figures now appear at the end of thesis. Added "Session RPE" to correlation and descriptives Table. Expanding theory, results and discussion sections.
</commit_message>
<xml_diff>
--- a/Markdown/References_BAEW.xlsx
+++ b/Markdown/References_BAEW.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28926"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_65A86265B625423E001F4B3DAFD6A80B062FC536" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7D5C29A-9F05-40A6-9DBC-C426DF498346}"/>
+  <xr:revisionPtr revIDLastSave="122" documentId="11_65A86265B625423E001F4B3DAFD6A80B062FC536" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{125F81AB-9733-46FA-81A6-9EF5C50A7BC1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21000" windowHeight="11655" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="233">
   <si>
     <t>@article{example2024,   title = {A Reference Example},   journal = {Journal of Examples},   publisher = {Example Press},   author = {Doe, Jane},   year = {2024},   month = aug,   pages = {185–209} }</t>
   </si>
@@ -1909,6 +1909,184 @@
 }</t>
   </si>
   <si>
+    <t xml:space="preserve">@article{Mueller2010,
+  author = {Müller, C. and Winter, C. and Rosenbaum, D.},
+  title = {{Aktuelle objektive Messverfahren zur Erfassung körperlicher Aktivität im Vergleich zu subjektiven Erhebungsmethoden: Current objective techniques for physical activity assessment in comparison with subjective methods}},
+  journal = {{Deutsche Zeitschrift für Sportmedizin}},
+  volume = {61},
+  number = {1},
+  year = {2010},
+  pages = {11--18},
+  url = {https://www.germanjournalsportsmedicine.com/fileadmin/content/archiv2010/heft01/11_uebersicht_mueller.pdf}
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@incollection{Eckert2014,
+  author = {Eckert, K. and Lange, M. and Wagner, P.},
+  title = {{Erfassung {k}{\"o}rperlicher {A}ktivit{\"a}t{\textendash}{E}in {{\"U}}berblick {\"u}ber {A}nspruch und {R}ealit{\"a}t einer validen {M}essung}},
+  booktitle = {{Aktiv und {G}esund? {I}nterdisziplin{\"a}re {P}erspektiven auf den {Z}usammenhang zwischen {S}port und {G}esundheit}},
+  editor = {},
+  pages = {97--124},
+  year = {2014},
+  publisher = {},
+  language = {de}
+}
+</t>
+  </si>
+  <si>
+    <t>@article{Vanhees2005,
+  title = {How to assess physical activity? How to assess physical fitness?},
+  volume = {12},
+  ISSN = {1741-8275},
+  url = {http://dx.doi.org/10.1097/01.hjr.0000161551.73095.9c},
+  DOI = {10.1097/01.hjr.0000161551.73095.9c},
+  number = {2},
+  journal = {European Journal of Cardiovascular Prevention &amp;amp; Rehabilitation},
+  publisher = {Oxford University Press (OUP)},
+  author = {Vanhees,  L. and Lefevre,  J. and Philippaerts,  R. and Martens,  M. and Huygens,  W. and Troosters,  T. and Beunen,  G.},
+  year = {2005},
+  month = apr,
+  pages = {102–114}
+}</t>
+  </si>
+  <si>
+    <t>@article{Kohl2000,
+  title = {Assessment of Physical Activity among Children and Adolescents: A Review and Synthesis},
+  volume = {31},
+  ISSN = {0091-7435},
+  url = {http://dx.doi.org/10.1006/pmed.1999.0542},
+  DOI = {10.1006/pmed.1999.0542},
+  number = {2},
+  journal = {Preventive Medicine},
+  publisher = {Elsevier BV},
+  author = {Kohl,  Harold W. and Fulton,  Janet E. and Caspersen,  Carl J.},
+  year = {2000},
+  month = aug,
+  pages = {S54–S76}
+}</t>
+  </si>
+  <si>
+    <t>@article{McLean2016,
+  title = {Quality and acceptability of measures of exercise adherence in musculoskeletal settings: a systematic review},
+  ISSN = {1462-0332},
+  url = {http://dx.doi.org/10.1093/rheumatology/kew422},
+  DOI = {10.1093/rheumatology/kew422},
+  journal = {Rheumatology},
+  publisher = {Oxford University Press (OUP)},
+  author = {McLean,  Sionnadh and Holden,  Melanie A. and Potia,  Tanzila and Gee,  Melanie and Mallett,  Ross and Bhanbhro,  Sadiq and Parsons,  Helen and Haywood,  Kirstie},
+  year = {2016},
+  month = dec,
+  pages = {kew422}
+}</t>
+  </si>
+  <si>
+    <t>@article{Duncan2002,
+  title = {Staying on Course: The Effects of an Adherence Facilitation Intervention on Home Exercise Participation},
+  volume = {17},
+  ISSN = {1751-7117},
+  url = {http://dx.doi.org/10.1111/j.0889-7204.2002.01229.x},
+  DOI = {10.1111/j.0889-7204.2002.01229.x},
+  number = {2},
+  journal = {Progress in Cardiovascular Nursing},
+  publisher = {Wiley},
+  author = {Duncan,  Kathleen A. and Pozehl,  Bunny},
+  year = {2002},
+  month = apr,
+  pages = {59–71}
+}</t>
+  </si>
+  <si>
+    <t>@article{Nigg2008,
+  title = {A Theory of Physical Activity Maintenance},
+  volume = {57},
+  ISSN = {1464-0597},
+  url = {http://dx.doi.org/10.1111/j.1464-0597.2008.00343.x},
+  DOI = {10.1111/j.1464-0597.2008.00343.x},
+  number = {4},
+  journal = {Applied Psychology},
+  publisher = {Wiley},
+  author = {Nigg,  Claudio R. and Borrelli,  Belinda and Maddock,  Jay and Dishman,  Rod K.},
+  year = {2008},
+  month = jul,
+  pages = {544–560}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@incollection{NationalAcademies2019,
+  author = {{National Academies of Sciences, Engineering, and Medicine}},
+  title = {Understanding Reproducibility and Replicability},
+  booktitle = {Reproducibility and Replicability in Science},
+  publisher = {National Academies Press},
+  address = {Washington, DC},
+  year = {2019},
+  chapter = {3},
+  url = {https://www.ncbi.nlm.nih.gov/books/NBK547546/},
+  note = {Committee on Reproducibility and Replicability in Science}
+}
+</t>
+  </si>
+  <si>
+    <t>@article{Yang2025,
+  title = {The role of affect regulation in health behavior change.},
+  ISSN = {0278-6133},
+  url = {http://dx.doi.org/10.1037/hea0001507},
+  DOI = {10.1037/hea0001507},
+  journal = {Health Psychology},
+  publisher = {American Psychological Association (APA)},
+  author = {Yang,  Michelle Z. and Conner,  Mark and Sheeran,  Paschal},
+  year = {2025},
+  month = apr 
+}</t>
+  </si>
+  <si>
+    <t>@article{Gratz2004,
+  title = {Multidimensional Assessment of Emotion Regulation and Dysregulation: Development,  Factor Structure,  and Initial Validation of the Difficulties in Emotion Regulation Scale},
+  volume = {26},
+  ISSN = {0882-2689},
+  url = {http://dx.doi.org/10.1023/B:JOBA.0000007455.08539.94},
+  DOI = {10.1023/b:joba.0000007455.08539.94},
+  number = {1},
+  journal = {Journal of Psychopathology and Behavioral Assessment},
+  publisher = {Springer Science and Business Media LLC},
+  author = {Gratz,  Kim L. and Roemer,  Lizabeth},
+  year = {2004},
+  month = mar,
+  pages = {41–54}
+}</t>
+  </si>
+  <si>
+    <t>@article{Buckholdt2014,
+  title = {Emotion Regulation Difficulties and Maladaptive Behaviors: Examination of Deliberate Self-harm,  Disordered Eating,  and Substance Misuse in Two Samples},
+  volume = {39},
+  ISSN = {1573-2819},
+  url = {http://dx.doi.org/10.1007/s10608-014-9655-3},
+  DOI = {10.1007/s10608-014-9655-3},
+  number = {2},
+  journal = {Cognitive Therapy and Research},
+  publisher = {Springer Science and Business Media LLC},
+  author = {Buckholdt,  Kelly E. and Parra,  Gilbert R. and Anestis,  Michael D. and Lavender,  Jason M. and Jobe-Shields,  Lisa E. and Tull,  Matthew T. and Gratz,  Kim L.},
+  year = {2014},
+  month = nov,
+  pages = {140–152}
+}</t>
+  </si>
+  <si>
+    <t>@article{Parfitt2009,
+  title = {The Exercise Intensity–Affect Relationship: Evidence and Implications for Exercise Behavior},
+  volume = {7},
+  ISSN = {1728-869X},
+  url = {http://dx.doi.org/10.1016/S1728-869X(09)60021-6},
+  DOI = {10.1016/s1728-869x(09)60021-6},
+  number = {2},
+  journal = {Journal of Exercise Science &amp;amp; Fitness},
+  publisher = {Elsevier BV},
+  author = {Parfitt,  Gaynor and Hughes,  Sophie},
+  year = {2009},
+  pages = {S34–S41}
+}</t>
+  </si>
+  <si>
     <t>Abbreviations</t>
   </si>
   <si>
@@ -2433,7 +2611,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2507,6 +2685,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -19049,8 +19230,8 @@
   <dimension ref="A1:R504"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A123" sqref="A123"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="15"/>
@@ -23360,386 +23541,410 @@
       <c r="I122" s="21"/>
     </row>
     <row r="123" spans="1:9" ht="36" customHeight="1">
-      <c r="A123" s="11"/>
+      <c r="A123" s="11" t="s">
+        <v>175</v>
+      </c>
       <c r="B123" s="12" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>@Mueller2010</v>
       </c>
       <c r="C123" s="13" t="str">
         <f t="shared" si="15"/>
-        <v>[]</v>
+        <v>[@Mueller2010]</v>
       </c>
       <c r="D123" s="14" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>2010</v>
       </c>
       <c r="E123" s="14" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>Müller, C. and Winter, C. and Rosenbaum, D.</v>
       </c>
       <c r="F123" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>{Aktuelle objektive Messverfahren zur Erfassung körperlicher Aktivität im Vergleich zu subjektiven Erhebungsmethoden: Current objective techniques for physical activity assessment in comparison with subjective methods}</v>
       </c>
       <c r="G123" s="16" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="H123" s="17" t="str">
+      <c r="H123" s="17">
         <f t="shared" ca="1" si="19"/>
-        <v/>
+        <v>45810.433583912039</v>
       </c>
       <c r="I123" s="21"/>
     </row>
     <row r="124" spans="1:9" ht="36" customHeight="1">
-      <c r="A124" s="11"/>
+      <c r="A124" s="11" t="s">
+        <v>176</v>
+      </c>
       <c r="B124" s="12" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>@Eckert2014</v>
       </c>
       <c r="C124" s="13" t="str">
         <f t="shared" si="15"/>
-        <v>[]</v>
+        <v>[@Eckert2014]</v>
       </c>
       <c r="D124" s="14" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>2014</v>
       </c>
       <c r="E124" s="14" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>Eckert, K. and Lange, M. and Wagner, P.</v>
       </c>
       <c r="F124" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>{Erfassung {k}{\"o}rperlicher {A}ktivit{\"a}t{\textendash}{E}in {{\"U}}berblick {\"u}ber {A}nspruch und {R}ealit{\"a}t einer validen {M}essung}</v>
       </c>
       <c r="G124" s="16" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="H124" s="17" t="str">
+      <c r="H124" s="17">
         <f t="shared" ca="1" si="19"/>
-        <v/>
+        <v>45810.442794097224</v>
       </c>
       <c r="I124" s="21"/>
     </row>
     <row r="125" spans="1:9" ht="36" customHeight="1">
-      <c r="A125" s="11"/>
+      <c r="A125" s="11" t="s">
+        <v>177</v>
+      </c>
       <c r="B125" s="12" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>@Vanhees2005</v>
       </c>
       <c r="C125" s="13" t="str">
         <f t="shared" si="15"/>
-        <v>[]</v>
+        <v>[@Vanhees2005]</v>
       </c>
       <c r="D125" s="14" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>2005</v>
       </c>
       <c r="E125" s="14" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>Vanhees,  L. and Lefevre,  J. and Philippaerts,  R. and Martens,  M. and Huygens,  W. and Troosters,  T. and Beunen,  G.</v>
       </c>
       <c r="F125" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>How to assess physical activity? How to assess physical fitness?</v>
       </c>
       <c r="G125" s="16" t="str">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="H125" s="17" t="str">
+        <v>https://doi.org/10.1097/01.hjr.0000161551.73095.9c</v>
+      </c>
+      <c r="H125" s="17">
         <f t="shared" ca="1" si="19"/>
-        <v/>
+        <v>45810.445725925929</v>
       </c>
       <c r="I125" s="21"/>
     </row>
     <row r="126" spans="1:9" ht="36" customHeight="1">
-      <c r="A126" s="11"/>
+      <c r="A126" s="11" t="s">
+        <v>178</v>
+      </c>
       <c r="B126" s="12" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>@Kohl2000</v>
       </c>
       <c r="C126" s="13" t="str">
         <f t="shared" si="15"/>
-        <v>[]</v>
+        <v>[@Kohl2000]</v>
       </c>
       <c r="D126" s="14" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>2000</v>
       </c>
       <c r="E126" s="14" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>Kohl,  Harold W. and Fulton,  Janet E. and Caspersen,  Carl J.</v>
       </c>
       <c r="F126" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>Assessment of Physical Activity among Children and Adolescents: A Review and Synthesis</v>
       </c>
       <c r="G126" s="16" t="str">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="H126" s="17" t="str">
+        <v>https://doi.org/10.1006/pmed.1999.0542</v>
+      </c>
+      <c r="H126" s="17">
         <f t="shared" ca="1" si="19"/>
-        <v/>
+        <v>45810.44733101852</v>
       </c>
       <c r="I126" s="21"/>
     </row>
     <row r="127" spans="1:9" ht="36" customHeight="1">
-      <c r="A127" s="11"/>
+      <c r="A127" s="11" t="s">
+        <v>179</v>
+      </c>
       <c r="B127" s="12" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>@McLean2016</v>
       </c>
       <c r="C127" s="13" t="str">
         <f t="shared" si="15"/>
-        <v>[]</v>
+        <v>[@McLean2016]</v>
       </c>
       <c r="D127" s="14" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>2016</v>
       </c>
       <c r="E127" s="14" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>McLean,  Sionnadh and Holden,  Melanie A. and Potia,  Tanzila and Gee,  Melanie and Mallett,  Ross and Bhanbhro,  Sadiq and Parsons,  Helen and Haywood,  Kirstie</v>
       </c>
       <c r="F127" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>Quality and acceptability of measures of exercise adherence in musculoskeletal settings: a systematic review</v>
       </c>
       <c r="G127" s="16" t="str">
         <f t="shared" si="18"/>
-        <v/>
-      </c>
-      <c r="H127" s="17" t="str">
+        <v>https://doi.org/10.1093/rheumatology/kew422</v>
+      </c>
+      <c r="H127" s="17">
         <f t="shared" ca="1" si="19"/>
-        <v/>
+        <v>45810.478872569445</v>
       </c>
       <c r="I127" s="21"/>
     </row>
     <row r="128" spans="1:9" ht="36" customHeight="1">
-      <c r="A128" s="11"/>
+      <c r="A128" s="11" t="s">
+        <v>180</v>
+      </c>
       <c r="B128" s="12" t="str">
         <f t="shared" ref="B128:B191" si="21">IFERROR("@"&amp;MID(A128,SEARCH("{",A128)+1,SEARCH(",",A128)-SEARCH("{",A128)-1),"")</f>
-        <v/>
+        <v>@Duncan2002</v>
       </c>
       <c r="C128" s="13" t="str">
         <f t="shared" ref="C128:C191" si="22">"["&amp;B128&amp;"]"</f>
-        <v>[]</v>
+        <v>[@Duncan2002]</v>
       </c>
       <c r="D128" s="14" t="str">
         <f t="shared" ref="D128:D191" si="23">IFERROR(MID(A128,SEARCH("year = {",A128)+8,4),"")</f>
-        <v/>
+        <v>2002</v>
       </c>
       <c r="E128" s="14" t="str">
         <f t="shared" ref="E128:E191" si="24">IFERROR(MID(A128,SEARCH("author = {",A128)+10,SEARCH("}",A128,SEARCH("author = {",A128))-SEARCH("author = {",A128)-10),"")</f>
-        <v/>
+        <v>Duncan,  Kathleen A. and Pozehl,  Bunny</v>
       </c>
       <c r="F128" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>Staying on Course: The Effects of an Adherence Facilitation Intervention on Home Exercise Participation</v>
       </c>
       <c r="G128" s="16" t="str">
         <f t="shared" ref="G128:G191" si="25">IFERROR("https://doi.org/"&amp;MID(A128,SEARCH("doi = {",A128)+7,FIND("}",A128,SEARCH("doi = {",A128))-SEARCH("doi = {",A128)-7),"")</f>
-        <v/>
-      </c>
-      <c r="H128" s="17" t="str">
+        <v>https://doi.org/10.1111/j.0889-7204.2002.01229.x</v>
+      </c>
+      <c r="H128" s="17">
         <f t="shared" ref="H128:H191" ca="1" si="26">IF(A128&lt;&gt;"",IF(H128&lt;&gt;"",H128,NOW()),"")</f>
-        <v/>
+        <v>45810.49402997685</v>
       </c>
       <c r="I128" s="21"/>
     </row>
     <row r="129" spans="1:9" ht="36" customHeight="1">
-      <c r="A129" s="11"/>
+      <c r="A129" s="11" t="s">
+        <v>181</v>
+      </c>
       <c r="B129" s="12" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>@Nigg2008</v>
       </c>
       <c r="C129" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>[]</v>
+        <v>[@Nigg2008]</v>
       </c>
       <c r="D129" s="14" t="str">
         <f t="shared" si="23"/>
-        <v/>
+        <v>2008</v>
       </c>
       <c r="E129" s="14" t="str">
         <f t="shared" si="24"/>
-        <v/>
+        <v>Nigg,  Claudio R. and Borrelli,  Belinda and Maddock,  Jay and Dishman,  Rod K.</v>
       </c>
       <c r="F129" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>A Theory of Physical Activity Maintenance</v>
       </c>
       <c r="G129" s="16" t="str">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="H129" s="17" t="str">
+        <v>https://doi.org/10.1111/j.1464-0597.2008.00343.x</v>
+      </c>
+      <c r="H129" s="17">
         <f t="shared" ca="1" si="26"/>
-        <v/>
+        <v>45810.494713657405</v>
       </c>
       <c r="I129" s="21"/>
     </row>
     <row r="130" spans="1:9" ht="36" customHeight="1">
-      <c r="A130" s="11"/>
+      <c r="A130" s="11" t="s">
+        <v>182</v>
+      </c>
       <c r="B130" s="12" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>@NationalAcademies2019</v>
       </c>
       <c r="C130" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>[]</v>
+        <v>[@NationalAcademies2019]</v>
       </c>
       <c r="D130" s="14" t="str">
         <f t="shared" si="23"/>
-        <v/>
+        <v>2019</v>
       </c>
       <c r="E130" s="14" t="str">
         <f t="shared" si="24"/>
-        <v/>
+        <v>{National Academies of Sciences, Engineering, and Medicine</v>
       </c>
       <c r="F130" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>Understanding Reproducibility and Replicability</v>
       </c>
       <c r="G130" s="16" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="H130" s="17" t="str">
+      <c r="H130" s="17">
         <f t="shared" ca="1" si="26"/>
-        <v/>
+        <v>45810.516860763892</v>
       </c>
       <c r="I130" s="21"/>
     </row>
     <row r="131" spans="1:9" ht="36" customHeight="1">
-      <c r="A131" s="11"/>
+      <c r="A131" s="11" t="s">
+        <v>183</v>
+      </c>
       <c r="B131" s="12" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>@Yang2025</v>
       </c>
       <c r="C131" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>[]</v>
+        <v>[@Yang2025]</v>
       </c>
       <c r="D131" s="14" t="str">
         <f t="shared" si="23"/>
-        <v/>
+        <v>2025</v>
       </c>
       <c r="E131" s="14" t="str">
         <f t="shared" si="24"/>
-        <v/>
+        <v>Yang,  Michelle Z. and Conner,  Mark and Sheeran,  Paschal</v>
       </c>
       <c r="F131" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>The role of affect regulation in health behavior change.</v>
       </c>
       <c r="G131" s="16" t="str">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="H131" s="17" t="str">
+        <v>https://doi.org/10.1037/hea0001507</v>
+      </c>
+      <c r="H131" s="17">
         <f t="shared" ca="1" si="26"/>
-        <v/>
+        <v>45810.856639351849</v>
       </c>
       <c r="I131" s="21"/>
     </row>
     <row r="132" spans="1:9" ht="36" customHeight="1">
-      <c r="A132" s="11"/>
+      <c r="A132" s="11" t="s">
+        <v>184</v>
+      </c>
       <c r="B132" s="12" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>@Gratz2004</v>
       </c>
       <c r="C132" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>[]</v>
+        <v>[@Gratz2004]</v>
       </c>
       <c r="D132" s="14" t="str">
         <f t="shared" si="23"/>
-        <v/>
+        <v>2004</v>
       </c>
       <c r="E132" s="14" t="str">
         <f t="shared" si="24"/>
-        <v/>
+        <v>Gratz,  Kim L. and Roemer,  Lizabeth</v>
       </c>
       <c r="F132" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>Multidimensional Assessment of Emotion Regulation and Dysregulation: Development,  Factor Structure,  and Initial Validation of the Difficulties in Emotion Regulation Scale</v>
       </c>
       <c r="G132" s="16" t="str">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="H132" s="17" t="str">
+        <v>https://doi.org/10.1023/b:joba.0000007455.08539.94</v>
+      </c>
+      <c r="H132" s="17">
         <f t="shared" ca="1" si="26"/>
-        <v/>
+        <v>45810.869453587962</v>
       </c>
       <c r="I132" s="21"/>
     </row>
     <row r="133" spans="1:9" ht="36" customHeight="1">
-      <c r="A133" s="11"/>
+      <c r="A133" s="11" t="s">
+        <v>185</v>
+      </c>
       <c r="B133" s="12" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>@Buckholdt2014</v>
       </c>
       <c r="C133" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>[]</v>
+        <v>[@Buckholdt2014]</v>
       </c>
       <c r="D133" s="14" t="str">
         <f t="shared" si="23"/>
-        <v/>
+        <v>2014</v>
       </c>
       <c r="E133" s="14" t="str">
         <f t="shared" si="24"/>
-        <v/>
+        <v>Buckholdt,  Kelly E. and Parra,  Gilbert R. and Anestis,  Michael D. and Lavender,  Jason M. and Jobe-Shields,  Lisa E. and Tull,  Matthew T. and Gratz,  Kim L.</v>
       </c>
       <c r="F133" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>Emotion Regulation Difficulties and Maladaptive Behaviors: Examination of Deliberate Self-harm,  Disordered Eating,  and Substance Misuse in Two Samples</v>
       </c>
       <c r="G133" s="16" t="str">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="H133" s="17" t="str">
+        <v>https://doi.org/10.1007/s10608-014-9655-3</v>
+      </c>
+      <c r="H133" s="17">
         <f t="shared" ca="1" si="26"/>
-        <v/>
+        <v>45810.871825115741</v>
       </c>
       <c r="I133" s="21"/>
     </row>
     <row r="134" spans="1:9" ht="36" customHeight="1">
-      <c r="A134" s="11"/>
+      <c r="A134" s="36" t="s">
+        <v>186</v>
+      </c>
       <c r="B134" s="12" t="str">
         <f t="shared" si="21"/>
-        <v/>
+        <v>@Parfitt2009</v>
       </c>
       <c r="C134" s="13" t="str">
         <f t="shared" si="22"/>
-        <v>[]</v>
+        <v>[@Parfitt2009]</v>
       </c>
       <c r="D134" s="14" t="str">
         <f t="shared" si="23"/>
-        <v/>
+        <v>2009</v>
       </c>
       <c r="E134" s="14" t="str">
         <f t="shared" si="24"/>
-        <v/>
+        <v>Parfitt,  Gaynor and Hughes,  Sophie</v>
       </c>
       <c r="F134" s="15" t="str">
         <f t="shared" si="20"/>
-        <v/>
+        <v>The Exercise Intensity–Affect Relationship: Evidence and Implications for Exercise Behavior</v>
       </c>
       <c r="G134" s="16" t="str">
         <f t="shared" si="25"/>
-        <v/>
-      </c>
-      <c r="H134" s="17" t="str">
+        <v>https://doi.org/10.1016/s1728-869x(09)60021-6</v>
+      </c>
+      <c r="H134" s="17">
         <f t="shared" ca="1" si="26"/>
-        <v/>
+        <v>45810.877912962962</v>
       </c>
       <c r="I134" s="21"/>
     </row>
@@ -35537,15 +35742,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="B2" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -35570,176 +35775,176 @@
   <sheetData>
     <row r="1" spans="1:3" ht="47.25" customHeight="1">
       <c r="A1" s="32" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="B1" s="32"/>
     </row>
     <row r="2" spans="1:3" ht="72.75" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="B2" s="34"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="35" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="B3" s="35"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="180" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="210" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="150" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>193</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="255" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="255" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>197</v>
+        <v>209</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="285" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="285" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="255" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="165" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="165" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="225" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="180" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="105" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="120" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="135" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>